<commit_message>
Completed Atomic DiagnosticReport profiles  - Diagnostic Report FHIR IG
Closes #50 Closes #53 Closes #21
</commit_message>
<xml_diff>
--- a/output/DiagnosticReport/diagnosticreport-imag-atomic-1.xlsx
+++ b/output/DiagnosticReport/diagnosticreport-imag-atomic-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2919" uniqueCount="502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2918" uniqueCount="503">
   <si>
     <t>Path</t>
   </si>
@@ -160,7 +160,7 @@
   </si>
   <si>
     <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}</t>
+dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}inv-dh-dir-01:The subject shall at least have a reference or an identifier with at least a system and a value {subject.reference.exists() or subject.identifier.where(system.count() + value.count() &gt;1).exists()}inv-dh-dir-02:The performer shall at least have a reference or an identifier with at least a system and a value {performer.reference.exists() or performer.identifier.where(system.count() + value.count() &gt;1).exists()}</t>
   </si>
   <si>
     <t>Event</t>
@@ -213,81 +213,85 @@
     <t>Resource.meta</t>
   </si>
   <si>
+    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+inv-dh-dir-03:One profile shall be 'http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/diagnosticreport-imag-atomic-1' {null}</t>
+  </si>
+  <si>
+    <t>DiagnosticReport.meta.id</t>
+  </si>
+  <si>
+    <t>Unique id for inter-element referencing</t>
+  </si>
+  <si>
+    <t>Unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
+  </si>
+  <si>
+    <t>Element.id</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>DiagnosticReport.meta.extension</t>
+  </si>
+  <si>
+    <t>extensions
+user content</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension
+</t>
+  </si>
+  <si>
+    <t>Additional content defined by implementations</t>
+  </si>
+  <si>
+    <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
+  </si>
+  <si>
+    <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value:url}
+</t>
+  </si>
+  <si>
+    <t>Extensions are always sliced by (at least) url</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>Element.extension</t>
+  </si>
+  <si>
+    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
+  </si>
+  <si>
+    <t>DiagnosticReport.meta.versionId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id
+</t>
+  </si>
+  <si>
+    <t>Version specific identifier</t>
+  </si>
+  <si>
+    <t>The version specific identifier, as it appears in the version portion of the URL. This value changes when the resource is created, updated, or deleted.</t>
+  </si>
+  <si>
+    <t>The server assigns this value, and ignores what the client specifies, except in the case that the server is imposing version integrity on updates/deletes.</t>
+  </si>
+  <si>
+    <t>Meta.versionId</t>
+  </si>
+  <si>
     <t xml:space="preserve">ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
 </t>
   </si>
   <si>
-    <t>DiagnosticReport.meta.id</t>
-  </si>
-  <si>
-    <t>Unique id for inter-element referencing</t>
-  </si>
-  <si>
-    <t>Unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
-  </si>
-  <si>
-    <t>Element.id</t>
-  </si>
-  <si>
-    <t>n/a</t>
-  </si>
-  <si>
-    <t>DiagnosticReport.meta.extension</t>
-  </si>
-  <si>
-    <t>extensions
-user content</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extension
-</t>
-  </si>
-  <si>
-    <t>Additional content defined by implementations</t>
-  </si>
-  <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
-  </si>
-  <si>
-    <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value:url}
-</t>
-  </si>
-  <si>
-    <t>Extensions are always sliced by (at least) url</t>
-  </si>
-  <si>
-    <t>open</t>
-  </si>
-  <si>
-    <t>Element.extension</t>
-  </si>
-  <si>
-    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
-  </si>
-  <si>
-    <t>DiagnosticReport.meta.versionId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">id
-</t>
-  </si>
-  <si>
-    <t>Version specific identifier</t>
-  </si>
-  <si>
-    <t>The version specific identifier, as it appears in the version portion of the URL. This value changes when the resource is created, updated, or deleted.</t>
-  </si>
-  <si>
-    <t>The server assigns this value, and ignores what the client specifies, except in the case that the server is imposing version integrity on updates/deletes.</t>
-  </si>
-  <si>
-    <t>Meta.versionId</t>
-  </si>
-  <si>
     <t>DiagnosticReport.meta.lastUpdated</t>
   </si>
   <si>
@@ -923,7 +927,7 @@
 </t>
   </si>
   <si>
-    <t>What was requested</t>
+    <t>Diagnostic imaging order</t>
   </si>
   <si>
     <t>Details concerning a service requested.</t>
@@ -1030,7 +1034,7 @@
     <t>DiagnosticReport.status</t>
   </si>
   <si>
-    <t>registered | partial | preliminary | final +</t>
+    <t>partial | preliminary | final +</t>
   </si>
   <si>
     <t>The status of the diagnostic report.</t>
@@ -1039,7 +1043,7 @@
     <t>Diagnostic services routinely issue provisional/incomplete reports, and sometimes withdraw previously released reports.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/diagnostic-report-status|4.0.1</t>
+    <t>https://healthterminologies.gov.au/fhir/ValueSet/diagnosticreportstatus-report-available-1</t>
   </si>
   <si>
     <t>Event.status</t>
@@ -1153,7 +1157,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/4.0/StructureDefinition/patient-mhr-1|http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/patient-ident-1)
+    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/patient-mhr-1|http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/patient-ident-1)
 </t>
   </si>
   <si>
@@ -1255,7 +1259,7 @@
 Date IssuedDate Verified</t>
   </si>
   <si>
-    <t>DateTime this version was made</t>
+    <t>Diagnostic imaging report date time</t>
   </si>
   <si>
     <t>The date and time that this version of the report was made available to providers, typically after the report was reviewed and verified.</t>
@@ -1283,7 +1287,7 @@
 ServicePractitionerDepartmentCompanyAuthorized byDirector</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/4.0/StructureDefinition/practitionerrole-ident-1|http://ns.electronichealth.net.au/ci/fhir/4.0/StructureDefinition/organization-ident-1)
+    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/practitionerrole-ident-1|http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/organization-ident-1)
 </t>
   </si>
   <si>
@@ -1768,7 +1772,7 @@
     <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="95.7734375" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="64.859375" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="82.98828125" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="40.03515625" customWidth="true" bestFit="true"/>
@@ -2551,7 +2555,7 @@
         <v>43</v>
       </c>
       <c r="AI7" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ7" t="s" s="2">
         <v>43</v>
@@ -2568,7 +2572,7 @@
     </row>
     <row r="8" hidden="true">
       <c r="A8" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s" s="2">
@@ -2591,16 +2595,16 @@
         <v>53</v>
       </c>
       <c r="J8" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K8" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="L8" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="M8" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="N8" s="2"/>
       <c r="O8" t="s" s="2">
@@ -2650,7 +2654,7 @@
         <v>43</v>
       </c>
       <c r="AE8" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AF8" t="s" s="2">
         <v>41</v>
@@ -2662,7 +2666,7 @@
         <v>43</v>
       </c>
       <c r="AI8" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ8" t="s" s="2">
         <v>43</v>
@@ -2679,7 +2683,7 @@
     </row>
     <row r="9" hidden="true">
       <c r="A9" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s" s="2">
@@ -2702,16 +2706,16 @@
         <v>53</v>
       </c>
       <c r="J9" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="K9" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L9" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="M9" t="s" s="2">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="N9" s="2"/>
       <c r="O9" t="s" s="2">
@@ -2761,7 +2765,7 @@
         <v>43</v>
       </c>
       <c r="AE9" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AF9" t="s" s="2">
         <v>41</v>
@@ -2773,7 +2777,7 @@
         <v>43</v>
       </c>
       <c r="AI9" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ9" t="s" s="2">
         <v>43</v>
@@ -2790,7 +2794,7 @@
     </row>
     <row r="10" hidden="true">
       <c r="A10" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s" s="2">
@@ -2813,16 +2817,16 @@
         <v>53</v>
       </c>
       <c r="J10" t="s" s="2">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="K10" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="L10" t="s" s="2">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="M10" t="s" s="2">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="N10" s="2"/>
       <c r="O10" t="s" s="2">
@@ -2872,7 +2876,7 @@
         <v>43</v>
       </c>
       <c r="AE10" t="s" s="2">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="AF10" t="s" s="2">
         <v>41</v>
@@ -2884,7 +2888,7 @@
         <v>43</v>
       </c>
       <c r="AI10" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ10" t="s" s="2">
         <v>43</v>
@@ -2901,7 +2905,7 @@
     </row>
     <row r="11" hidden="true">
       <c r="A11" t="s" s="2">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s" s="2">
@@ -2924,16 +2928,16 @@
         <v>53</v>
       </c>
       <c r="J11" t="s" s="2">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="K11" t="s" s="2">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="L11" t="s" s="2">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="M11" t="s" s="2">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="N11" s="2"/>
       <c r="O11" t="s" s="2">
@@ -2959,13 +2963,13 @@
         <v>43</v>
       </c>
       <c r="W11" t="s" s="2">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="X11" t="s" s="2">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="Y11" t="s" s="2">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="Z11" t="s" s="2">
         <v>43</v>
@@ -2983,7 +2987,7 @@
         <v>43</v>
       </c>
       <c r="AE11" t="s" s="2">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AF11" t="s" s="2">
         <v>41</v>
@@ -2995,7 +2999,7 @@
         <v>43</v>
       </c>
       <c r="AI11" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ11" t="s" s="2">
         <v>43</v>
@@ -3012,7 +3016,7 @@
     </row>
     <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s" s="2">
@@ -3035,16 +3039,16 @@
         <v>53</v>
       </c>
       <c r="J12" t="s" s="2">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="M12" t="s" s="2">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="N12" s="2"/>
       <c r="O12" t="s" s="2">
@@ -3070,13 +3074,13 @@
         <v>43</v>
       </c>
       <c r="W12" t="s" s="2">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="X12" t="s" s="2">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="Y12" t="s" s="2">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="Z12" t="s" s="2">
         <v>43</v>
@@ -3094,7 +3098,7 @@
         <v>43</v>
       </c>
       <c r="AE12" t="s" s="2">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="AF12" t="s" s="2">
         <v>41</v>
@@ -3106,7 +3110,7 @@
         <v>43</v>
       </c>
       <c r="AI12" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ12" t="s" s="2">
         <v>43</v>
@@ -3123,7 +3127,7 @@
     </row>
     <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
@@ -3146,16 +3150,16 @@
         <v>53</v>
       </c>
       <c r="J13" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="M13" t="s" s="2">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="N13" s="2"/>
       <c r="O13" t="s" s="2">
@@ -3205,7 +3209,7 @@
         <v>43</v>
       </c>
       <c r="AE13" t="s" s="2">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AF13" t="s" s="2">
         <v>41</v>
@@ -3217,7 +3221,7 @@
         <v>43</v>
       </c>
       <c r="AI13" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ13" t="s" s="2">
         <v>43</v>
@@ -3234,7 +3238,7 @@
     </row>
     <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
@@ -3257,16 +3261,16 @@
         <v>43</v>
       </c>
       <c r="J14" t="s" s="2">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="M14" t="s" s="2">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="N14" s="2"/>
       <c r="O14" t="s" s="2">
@@ -3274,7 +3278,7 @@
       </c>
       <c r="P14" s="2"/>
       <c r="Q14" t="s" s="2">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="R14" t="s" s="2">
         <v>43</v>
@@ -3292,13 +3296,13 @@
         <v>43</v>
       </c>
       <c r="W14" t="s" s="2">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="X14" t="s" s="2">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="Y14" t="s" s="2">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="Z14" t="s" s="2">
         <v>43</v>
@@ -3316,7 +3320,7 @@
         <v>43</v>
       </c>
       <c r="AE14" t="s" s="2">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="AF14" t="s" s="2">
         <v>41</v>
@@ -3328,7 +3332,7 @@
         <v>43</v>
       </c>
       <c r="AI14" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ14" t="s" s="2">
         <v>43</v>
@@ -3345,11 +3349,11 @@
     </row>
     <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" t="s" s="2">
@@ -3368,16 +3372,16 @@
         <v>43</v>
       </c>
       <c r="J15" t="s" s="2">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="M15" t="s" s="2">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="N15" s="2"/>
       <c r="O15" t="s" s="2">
@@ -3427,7 +3431,7 @@
         <v>43</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="AF15" t="s" s="2">
         <v>41</v>
@@ -3439,7 +3443,7 @@
         <v>43</v>
       </c>
       <c r="AI15" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ15" t="s" s="2">
         <v>43</v>
@@ -3448,7 +3452,7 @@
         <v>43</v>
       </c>
       <c r="AL15" t="s" s="2">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="AM15" t="s" s="2">
         <v>43</v>
@@ -3456,11 +3460,11 @@
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" t="s" s="2">
@@ -3479,16 +3483,16 @@
         <v>43</v>
       </c>
       <c r="J16" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="M16" t="s" s="2">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="N16" s="2"/>
       <c r="O16" t="s" s="2">
@@ -3538,7 +3542,7 @@
         <v>43</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="AF16" t="s" s="2">
         <v>41</v>
@@ -3559,7 +3563,7 @@
         <v>43</v>
       </c>
       <c r="AL16" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AM16" t="s" s="2">
         <v>43</v>
@@ -3567,7 +3571,7 @@
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
@@ -3596,7 +3600,7 @@
         <v>73</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="M17" t="s" s="2">
         <v>75</v>
@@ -3649,7 +3653,7 @@
         <v>43</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>41</v>
@@ -3670,7 +3674,7 @@
         <v>43</v>
       </c>
       <c r="AL17" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AM17" t="s" s="2">
         <v>43</v>
@@ -3678,7 +3682,7 @@
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
@@ -3704,16 +3708,16 @@
         <v>72</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="M18" t="s" s="2">
         <v>75</v>
       </c>
       <c r="N18" t="s" s="2">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="O18" t="s" s="2">
         <v>43</v>
@@ -3762,7 +3766,7 @@
         <v>43</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>41</v>
@@ -3783,7 +3787,7 @@
         <v>43</v>
       </c>
       <c r="AL18" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AM18" t="s" s="2">
         <v>43</v>
@@ -3791,11 +3795,11 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" t="s" s="2">
@@ -3814,19 +3818,19 @@
         <v>53</v>
       </c>
       <c r="J19" t="s" s="2">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="N19" t="s" s="2">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="O19" t="s" s="2">
         <v>43</v>
@@ -3863,7 +3867,7 @@
         <v>43</v>
       </c>
       <c r="AA19" t="s" s="2">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="AB19" s="2"/>
       <c r="AC19" t="s" s="2">
@@ -3873,7 +3877,7 @@
         <v>78</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>41</v>
@@ -3885,30 +3889,30 @@
         <v>43</v>
       </c>
       <c r="AI19" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ19" t="s" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="AK19" t="s" s="2">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="AL19" t="s" s="2">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="AM19" t="s" s="2">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C20" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" t="s" s="2">
@@ -3927,19 +3931,19 @@
         <v>53</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="N20" t="s" s="2">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="O20" t="s" s="2">
         <v>43</v>
@@ -3988,7 +3992,7 @@
         <v>43</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>41</v>
@@ -4000,24 +4004,24 @@
         <v>43</v>
       </c>
       <c r="AI20" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ20" t="s" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="AL20" t="s" s="2">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="AM20" t="s" s="2">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -4126,7 +4130,7 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
@@ -4237,7 +4241,7 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -4260,19 +4264,19 @@
         <v>53</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="N23" t="s" s="2">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="O23" t="s" s="2">
         <v>43</v>
@@ -4297,13 +4301,13 @@
         <v>43</v>
       </c>
       <c r="W23" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="X23" t="s" s="2">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="Y23" t="s" s="2">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="Z23" t="s" s="2">
         <v>43</v>
@@ -4321,7 +4325,7 @@
         <v>43</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>41</v>
@@ -4333,16 +4337,16 @@
         <v>43</v>
       </c>
       <c r="AI23" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ23" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="AM23" t="s" s="2">
         <v>43</v>
@@ -4350,7 +4354,7 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -4373,19 +4377,19 @@
         <v>53</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="N24" t="s" s="2">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="O24" t="s" s="2">
         <v>43</v>
@@ -4410,11 +4414,11 @@
         <v>43</v>
       </c>
       <c r="W24" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="X24" s="2"/>
       <c r="Y24" t="s" s="2">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="Z24" t="s" s="2">
         <v>43</v>
@@ -4432,7 +4436,7 @@
         <v>43</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>41</v>
@@ -4444,16 +4448,16 @@
         <v>43</v>
       </c>
       <c r="AI24" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ24" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="AL24" t="s" s="2">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="AM24" t="s" s="2">
         <v>43</v>
@@ -4461,7 +4465,7 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -4570,7 +4574,7 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -4681,7 +4685,7 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -4704,19 +4708,19 @@
         <v>53</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="N27" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="O27" t="s" s="2">
         <v>43</v>
@@ -4765,7 +4769,7 @@
         <v>43</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>41</v>
@@ -4777,16 +4781,16 @@
         <v>43</v>
       </c>
       <c r="AI27" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ27" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="AM27" t="s" s="2">
         <v>43</v>
@@ -4794,7 +4798,7 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4903,7 +4907,7 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -5014,7 +5018,7 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -5037,26 +5041,26 @@
         <v>53</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="N30" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="O30" t="s" s="2">
         <v>43</v>
       </c>
       <c r="P30" s="2"/>
       <c r="Q30" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="R30" t="s" s="2">
         <v>43</v>
@@ -5098,7 +5102,7 @@
         <v>43</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>41</v>
@@ -5110,16 +5114,16 @@
         <v>43</v>
       </c>
       <c r="AI30" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ30" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="AM30" t="s" s="2">
         <v>43</v>
@@ -5127,7 +5131,7 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -5153,13 +5157,13 @@
         <v>54</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
@@ -5209,7 +5213,7 @@
         <v>43</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>41</v>
@@ -5221,16 +5225,16 @@
         <v>43</v>
       </c>
       <c r="AI31" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ31" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="AM31" t="s" s="2">
         <v>43</v>
@@ -5238,7 +5242,7 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -5261,24 +5265,24 @@
         <v>53</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="M32" s="2"/>
       <c r="N32" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="O32" t="s" s="2">
         <v>43</v>
       </c>
       <c r="P32" s="2"/>
       <c r="Q32" t="s" s="2">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="R32" t="s" s="2">
         <v>43</v>
@@ -5320,7 +5324,7 @@
         <v>43</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>41</v>
@@ -5332,16 +5336,16 @@
         <v>43</v>
       </c>
       <c r="AI32" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ32" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK32" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="AM32" t="s" s="2">
         <v>43</v>
@@ -5349,7 +5353,7 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -5375,14 +5379,14 @@
         <v>54</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="M33" s="2"/>
       <c r="N33" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="O33" t="s" s="2">
         <v>43</v>
@@ -5431,7 +5435,7 @@
         <v>43</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>41</v>
@@ -5443,16 +5447,16 @@
         <v>43</v>
       </c>
       <c r="AI33" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ33" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK33" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="AM33" t="s" s="2">
         <v>43</v>
@@ -5460,7 +5464,7 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -5483,19 +5487,19 @@
         <v>53</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="N34" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="O34" t="s" s="2">
         <v>43</v>
@@ -5544,7 +5548,7 @@
         <v>43</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>41</v>
@@ -5556,16 +5560,16 @@
         <v>43</v>
       </c>
       <c r="AI34" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ34" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK34" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AM34" t="s" s="2">
         <v>43</v>
@@ -5573,7 +5577,7 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5599,16 +5603,16 @@
         <v>54</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="N35" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="O35" t="s" s="2">
         <v>43</v>
@@ -5657,7 +5661,7 @@
         <v>43</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>41</v>
@@ -5669,16 +5673,16 @@
         <v>43</v>
       </c>
       <c r="AI35" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ35" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK35" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AM35" t="s" s="2">
         <v>43</v>
@@ -5686,7 +5690,7 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5709,19 +5713,19 @@
         <v>53</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="N36" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="O36" t="s" s="2">
         <v>43</v>
@@ -5734,7 +5738,7 @@
         <v>43</v>
       </c>
       <c r="S36" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="T36" t="s" s="2">
         <v>43</v>
@@ -5770,7 +5774,7 @@
         <v>43</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>41</v>
@@ -5782,16 +5786,16 @@
         <v>43</v>
       </c>
       <c r="AI36" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ36" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AM36" t="s" s="2">
         <v>43</v>
@@ -5799,7 +5803,7 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5825,13 +5829,13 @@
         <v>54</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="N37" s="2"/>
       <c r="O37" t="s" s="2">
@@ -5845,7 +5849,7 @@
         <v>43</v>
       </c>
       <c r="S37" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="T37" t="s" s="2">
         <v>43</v>
@@ -5881,7 +5885,7 @@
         <v>43</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>41</v>
@@ -5893,16 +5897,16 @@
         <v>43</v>
       </c>
       <c r="AI37" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ37" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK37" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="AM37" t="s" s="2">
         <v>43</v>
@@ -5910,7 +5914,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5933,13 +5937,13 @@
         <v>53</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
@@ -5990,7 +5994,7 @@
         <v>43</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>41</v>
@@ -6002,16 +6006,16 @@
         <v>43</v>
       </c>
       <c r="AI38" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ38" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="AM38" t="s" s="2">
         <v>43</v>
@@ -6019,7 +6023,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -6042,16 +6046,16 @@
         <v>53</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="N39" s="2"/>
       <c r="O39" t="s" s="2">
@@ -6101,7 +6105,7 @@
         <v>43</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>41</v>
@@ -6113,16 +6117,16 @@
         <v>43</v>
       </c>
       <c r="AI39" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ39" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="AM39" t="s" s="2">
         <v>43</v>
@@ -6130,11 +6134,11 @@
     </row>
     <row r="40">
       <c r="A40" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" t="s" s="2">
@@ -6153,19 +6157,19 @@
         <v>43</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="N40" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="O40" t="s" s="2">
         <v>43</v>
@@ -6214,7 +6218,7 @@
         <v>43</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>41</v>
@@ -6226,16 +6230,16 @@
         <v>43</v>
       </c>
       <c r="AI40" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ40" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="AM40" t="s" s="2">
         <v>43</v>
@@ -6243,7 +6247,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -6352,7 +6356,7 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -6463,7 +6467,7 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6489,13 +6493,13 @@
         <v>54</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="N43" s="2"/>
       <c r="O43" t="s" s="2">
@@ -6545,7 +6549,7 @@
         <v>43</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>41</v>
@@ -6554,10 +6558,10 @@
         <v>52</v>
       </c>
       <c r="AH43" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="AI43" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ43" t="s" s="2">
         <v>43</v>
@@ -6566,7 +6570,7 @@
         <v>43</v>
       </c>
       <c r="AL43" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AM43" t="s" s="2">
         <v>43</v>
@@ -6574,7 +6578,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6597,16 +6601,16 @@
         <v>53</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="N44" s="2"/>
       <c r="O44" t="s" s="2">
@@ -6632,13 +6636,13 @@
         <v>43</v>
       </c>
       <c r="W44" t="s" s="2">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="X44" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="Y44" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="Z44" t="s" s="2">
         <v>43</v>
@@ -6656,7 +6660,7 @@
         <v>43</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>41</v>
@@ -6668,7 +6672,7 @@
         <v>43</v>
       </c>
       <c r="AI44" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ44" t="s" s="2">
         <v>43</v>
@@ -6677,7 +6681,7 @@
         <v>43</v>
       </c>
       <c r="AL44" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AM44" t="s" s="2">
         <v>43</v>
@@ -6685,7 +6689,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6708,16 +6712,16 @@
         <v>53</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="N45" s="2"/>
       <c r="O45" t="s" s="2">
@@ -6767,7 +6771,7 @@
         <v>43</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>41</v>
@@ -6779,7 +6783,7 @@
         <v>43</v>
       </c>
       <c r="AI45" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ45" t="s" s="2">
         <v>43</v>
@@ -6788,7 +6792,7 @@
         <v>43</v>
       </c>
       <c r="AL45" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="AM45" t="s" s="2">
         <v>43</v>
@@ -6796,7 +6800,7 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -6822,13 +6826,13 @@
         <v>54</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="N46" s="2"/>
       <c r="O46" t="s" s="2">
@@ -6878,7 +6882,7 @@
         <v>43</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>41</v>
@@ -6890,7 +6894,7 @@
         <v>43</v>
       </c>
       <c r="AI46" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ46" t="s" s="2">
         <v>43</v>
@@ -6899,7 +6903,7 @@
         <v>43</v>
       </c>
       <c r="AL46" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AM46" t="s" s="2">
         <v>43</v>
@@ -6907,7 +6911,7 @@
     </row>
     <row r="47">
       <c r="A47" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -6930,17 +6934,17 @@
         <v>53</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="M47" s="2"/>
       <c r="N47" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="O47" t="s" s="2">
         <v>43</v>
@@ -6965,13 +6969,11 @@
         <v>43</v>
       </c>
       <c r="W47" t="s" s="2">
-        <v>183</v>
-      </c>
-      <c r="X47" t="s" s="2">
-        <v>327</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="X47" s="2"/>
       <c r="Y47" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="Z47" t="s" s="2">
         <v>43</v>
@@ -6989,7 +6991,7 @@
         <v>43</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>52</v>
@@ -7001,28 +7003,28 @@
         <v>43</v>
       </c>
       <c r="AI47" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ47" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="AK47" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="AL47" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" t="s" s="2">
@@ -7041,16 +7043,16 @@
         <v>53</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="N48" s="2"/>
       <c r="O48" t="s" s="2">
@@ -7061,7 +7063,7 @@
         <v>43</v>
       </c>
       <c r="R48" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="S48" t="s" s="2">
         <v>43</v>
@@ -7076,11 +7078,11 @@
         <v>43</v>
       </c>
       <c r="W48" t="s" s="2">
-        <v>133</v>
+        <v>111</v>
       </c>
       <c r="X48" s="2"/>
       <c r="Y48" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="Z48" t="s" s="2">
         <v>43</v>
@@ -7098,7 +7100,7 @@
         <v>43</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>41</v>
@@ -7110,28 +7112,28 @@
         <v>43</v>
       </c>
       <c r="AI48" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ48" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="AL48" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" t="s" s="2">
@@ -7150,13 +7152,13 @@
         <v>53</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
@@ -7183,13 +7185,13 @@
         <v>43</v>
       </c>
       <c r="W49" t="s" s="2">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="X49" t="s" s="2">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="Y49" t="s" s="2">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="Z49" t="s" s="2">
         <v>43</v>
@@ -7207,7 +7209,7 @@
         <v>43</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>52</v>
@@ -7219,24 +7221,24 @@
         <v>43</v>
       </c>
       <c r="AI49" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ49" t="s" s="2">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -7345,7 +7347,7 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -7456,7 +7458,7 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -7479,19 +7481,19 @@
         <v>53</v>
       </c>
       <c r="J52" t="s" s="2">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="N52" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="O52" t="s" s="2">
         <v>43</v>
@@ -7528,7 +7530,7 @@
         <v>43</v>
       </c>
       <c r="AA52" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="AB52" s="2"/>
       <c r="AC52" t="s" s="2">
@@ -7538,7 +7540,7 @@
         <v>78</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>41</v>
@@ -7550,16 +7552,16 @@
         <v>43</v>
       </c>
       <c r="AI52" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ52" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK52" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="AL52" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="AM52" t="s" s="2">
         <v>43</v>
@@ -7567,10 +7569,10 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B53" t="s" s="2">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C53" t="s" s="2">
         <v>43</v>
@@ -7592,19 +7594,19 @@
         <v>53</v>
       </c>
       <c r="J53" t="s" s="2">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="M53" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="N53" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="O53" t="s" s="2">
         <v>43</v>
@@ -7629,11 +7631,11 @@
         <v>43</v>
       </c>
       <c r="W53" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="X53" s="2"/>
       <c r="Y53" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="Z53" t="s" s="2">
         <v>43</v>
@@ -7651,7 +7653,7 @@
         <v>43</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>41</v>
@@ -7663,16 +7665,16 @@
         <v>43</v>
       </c>
       <c r="AI53" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ53" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK53" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="AL53" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="AM53" t="s" s="2">
         <v>43</v>
@@ -7680,7 +7682,7 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -7706,16 +7708,16 @@
         <v>54</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="M54" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="N54" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="O54" t="s" s="2">
         <v>43</v>
@@ -7764,7 +7766,7 @@
         <v>43</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>41</v>
@@ -7776,16 +7778,16 @@
         <v>43</v>
       </c>
       <c r="AI54" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ54" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK54" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AL54" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AM54" t="s" s="2">
         <v>43</v>
@@ -7793,11 +7795,11 @@
     </row>
     <row r="55">
       <c r="A55" t="s" s="2">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" t="s" s="2">
@@ -7816,17 +7818,17 @@
         <v>53</v>
       </c>
       <c r="J55" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="M55" s="2"/>
       <c r="N55" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="O55" t="s" s="2">
         <v>43</v>
@@ -7875,7 +7877,7 @@
         <v>43</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>41</v>
@@ -7887,28 +7889,28 @@
         <v>43</v>
       </c>
       <c r="AI55" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ55" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="AK55" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="AL55" t="s" s="2">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="AM55" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" t="s" s="2">
@@ -7927,19 +7929,19 @@
         <v>53</v>
       </c>
       <c r="J56" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="M56" t="s" s="2">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="N56" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="O56" t="s" s="2">
         <v>43</v>
@@ -7988,7 +7990,7 @@
         <v>43</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>41</v>
@@ -8000,28 +8002,28 @@
         <v>43</v>
       </c>
       <c r="AI56" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ56" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="AK56" t="s" s="2">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="AL56" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="AM56" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" t="s" s="2">
@@ -8040,19 +8042,19 @@
         <v>53</v>
       </c>
       <c r="J57" t="s" s="2">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="M57" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="N57" t="s" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="O57" t="s" s="2">
         <v>43</v>
@@ -8101,7 +8103,7 @@
         <v>43</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>41</v>
@@ -8113,28 +8115,28 @@
         <v>43</v>
       </c>
       <c r="AI57" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ57" t="s" s="2">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="AK57" t="s" s="2">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="AL57" t="s" s="2">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="AM57" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="2">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" t="s" s="2">
@@ -8153,19 +8155,19 @@
         <v>53</v>
       </c>
       <c r="J58" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="M58" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="N58" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="O58" t="s" s="2">
         <v>43</v>
@@ -8214,7 +8216,7 @@
         <v>43</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>41</v>
@@ -8226,28 +8228,28 @@
         <v>43</v>
       </c>
       <c r="AI58" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ58" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK58" t="s" s="2">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="AL58" t="s" s="2">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="AM58" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="2">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" t="s" s="2">
@@ -8266,19 +8268,19 @@
         <v>53</v>
       </c>
       <c r="J59" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="M59" t="s" s="2">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="N59" t="s" s="2">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="O59" t="s" s="2">
         <v>43</v>
@@ -8327,7 +8329,7 @@
         <v>43</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>41</v>
@@ -8339,28 +8341,28 @@
         <v>43</v>
       </c>
       <c r="AI59" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ59" t="s" s="2">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="AK59" t="s" s="2">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="AL59" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="AM59" t="s" s="2">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" t="s" s="2">
@@ -8379,19 +8381,19 @@
         <v>53</v>
       </c>
       <c r="J60" t="s" s="2">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="M60" t="s" s="2">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="N60" t="s" s="2">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="O60" t="s" s="2">
         <v>43</v>
@@ -8440,7 +8442,7 @@
         <v>43</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>41</v>
@@ -8452,24 +8454,24 @@
         <v>43</v>
       </c>
       <c r="AI60" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ60" t="s" s="2">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="AK60" t="s" s="2">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="AL60" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="AM60" t="s" s="2">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
@@ -8492,19 +8494,19 @@
         <v>43</v>
       </c>
       <c r="J61" t="s" s="2">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="M61" t="s" s="2">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="N61" t="s" s="2">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="O61" t="s" s="2">
         <v>43</v>
@@ -8553,7 +8555,7 @@
         <v>43</v>
       </c>
       <c r="AE61" t="s" s="2">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="AF61" t="s" s="2">
         <v>41</v>
@@ -8565,16 +8567,16 @@
         <v>43</v>
       </c>
       <c r="AI61" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ61" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK61" t="s" s="2">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="AL61" t="s" s="2">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="AM61" t="s" s="2">
         <v>43</v>
@@ -8582,11 +8584,11 @@
     </row>
     <row r="62">
       <c r="A62" t="s" s="2">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" t="s" s="2">
@@ -8605,19 +8607,19 @@
         <v>43</v>
       </c>
       <c r="J62" t="s" s="2">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="M62" t="s" s="2">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="N62" t="s" s="2">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="O62" t="s" s="2">
         <v>43</v>
@@ -8666,7 +8668,7 @@
         <v>43</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>41</v>
@@ -8678,16 +8680,16 @@
         <v>43</v>
       </c>
       <c r="AI62" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ62" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK62" t="s" s="2">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="AL62" t="s" s="2">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="AM62" t="s" s="2">
         <v>43</v>
@@ -8695,7 +8697,7 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
@@ -8804,7 +8806,7 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
@@ -8915,7 +8917,7 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
@@ -8941,13 +8943,13 @@
         <v>54</v>
       </c>
       <c r="K65" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="L65" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="M65" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="N65" s="2"/>
       <c r="O65" t="s" s="2">
@@ -8997,7 +8999,7 @@
         <v>43</v>
       </c>
       <c r="AE65" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="AF65" t="s" s="2">
         <v>41</v>
@@ -9006,10 +9008,10 @@
         <v>52</v>
       </c>
       <c r="AH65" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="AI65" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ65" t="s" s="2">
         <v>43</v>
@@ -9018,7 +9020,7 @@
         <v>43</v>
       </c>
       <c r="AL65" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AM65" t="s" s="2">
         <v>43</v>
@@ -9026,7 +9028,7 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
@@ -9049,16 +9051,16 @@
         <v>53</v>
       </c>
       <c r="J66" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="K66" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="M66" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="N66" s="2"/>
       <c r="O66" t="s" s="2">
@@ -9084,13 +9086,13 @@
         <v>43</v>
       </c>
       <c r="W66" t="s" s="2">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="X66" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="Y66" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="Z66" t="s" s="2">
         <v>43</v>
@@ -9108,7 +9110,7 @@
         <v>43</v>
       </c>
       <c r="AE66" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="AF66" t="s" s="2">
         <v>41</v>
@@ -9120,7 +9122,7 @@
         <v>43</v>
       </c>
       <c r="AI66" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ66" t="s" s="2">
         <v>43</v>
@@ -9129,7 +9131,7 @@
         <v>43</v>
       </c>
       <c r="AL66" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AM66" t="s" s="2">
         <v>43</v>
@@ -9137,7 +9139,7 @@
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" t="s" s="2">
@@ -9160,16 +9162,16 @@
         <v>53</v>
       </c>
       <c r="J67" t="s" s="2">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="K67" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="L67" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="M67" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="N67" s="2"/>
       <c r="O67" t="s" s="2">
@@ -9219,7 +9221,7 @@
         <v>43</v>
       </c>
       <c r="AE67" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="AF67" t="s" s="2">
         <v>41</v>
@@ -9231,7 +9233,7 @@
         <v>43</v>
       </c>
       <c r="AI67" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ67" t="s" s="2">
         <v>43</v>
@@ -9240,7 +9242,7 @@
         <v>43</v>
       </c>
       <c r="AL67" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="AM67" t="s" s="2">
         <v>43</v>
@@ -9248,7 +9250,7 @@
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" t="s" s="2">
@@ -9274,13 +9276,13 @@
         <v>54</v>
       </c>
       <c r="K68" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="L68" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="M68" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="N68" s="2"/>
       <c r="O68" t="s" s="2">
@@ -9330,7 +9332,7 @@
         <v>43</v>
       </c>
       <c r="AE68" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="AF68" t="s" s="2">
         <v>41</v>
@@ -9342,7 +9344,7 @@
         <v>43</v>
       </c>
       <c r="AI68" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ68" t="s" s="2">
         <v>43</v>
@@ -9351,7 +9353,7 @@
         <v>43</v>
       </c>
       <c r="AL68" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AM68" t="s" s="2">
         <v>43</v>
@@ -9359,7 +9361,7 @@
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" t="s" s="2">
@@ -9382,16 +9384,16 @@
         <v>43</v>
       </c>
       <c r="J69" t="s" s="2">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="K69" t="s" s="2">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="L69" t="s" s="2">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="M69" t="s" s="2">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="N69" s="2"/>
       <c r="O69" t="s" s="2">
@@ -9441,7 +9443,7 @@
         <v>43</v>
       </c>
       <c r="AE69" t="s" s="2">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="AF69" t="s" s="2">
         <v>41</v>
@@ -9453,7 +9455,7 @@
         <v>43</v>
       </c>
       <c r="AI69" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ69" t="s" s="2">
         <v>43</v>
@@ -9462,7 +9464,7 @@
         <v>43</v>
       </c>
       <c r="AL69" t="s" s="2">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="AM69" t="s" s="2">
         <v>43</v>
@@ -9470,11 +9472,11 @@
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" t="s" s="2">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="D70" s="2"/>
       <c r="E70" t="s" s="2">
@@ -9493,17 +9495,17 @@
         <v>53</v>
       </c>
       <c r="J70" t="s" s="2">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="K70" t="s" s="2">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="L70" t="s" s="2">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="M70" s="2"/>
       <c r="N70" t="s" s="2">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="O70" t="s" s="2">
         <v>43</v>
@@ -9552,7 +9554,7 @@
         <v>43</v>
       </c>
       <c r="AE70" t="s" s="2">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="AF70" t="s" s="2">
         <v>41</v>
@@ -9564,16 +9566,16 @@
         <v>43</v>
       </c>
       <c r="AI70" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ70" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK70" t="s" s="2">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="AL70" t="s" s="2">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="AM70" t="s" s="2">
         <v>43</v>
@@ -9581,7 +9583,7 @@
     </row>
     <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" t="s" s="2">
@@ -9690,7 +9692,7 @@
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" t="s" s="2">
@@ -9801,11 +9803,11 @@
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" t="s" s="2">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="D73" s="2"/>
       <c r="E73" t="s" s="2">
@@ -9827,16 +9829,16 @@
         <v>72</v>
       </c>
       <c r="K73" t="s" s="2">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="L73" t="s" s="2">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="M73" t="s" s="2">
         <v>75</v>
       </c>
       <c r="N73" t="s" s="2">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="O73" t="s" s="2">
         <v>43</v>
@@ -9885,7 +9887,7 @@
         <v>43</v>
       </c>
       <c r="AE73" t="s" s="2">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="AF73" t="s" s="2">
         <v>41</v>
@@ -9906,7 +9908,7 @@
         <v>43</v>
       </c>
       <c r="AL73" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AM73" t="s" s="2">
         <v>43</v>
@@ -9914,7 +9916,7 @@
     </row>
     <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" t="s" s="2">
@@ -9940,16 +9942,16 @@
         <v>54</v>
       </c>
       <c r="K74" t="s" s="2">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="L74" t="s" s="2">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="M74" t="s" s="2">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="N74" t="s" s="2">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="O74" t="s" s="2">
         <v>43</v>
@@ -9998,7 +10000,7 @@
         <v>43</v>
       </c>
       <c r="AE74" t="s" s="2">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="AF74" t="s" s="2">
         <v>41</v>
@@ -10010,7 +10012,7 @@
         <v>43</v>
       </c>
       <c r="AI74" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ74" t="s" s="2">
         <v>43</v>
@@ -10019,7 +10021,7 @@
         <v>43</v>
       </c>
       <c r="AL74" t="s" s="2">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="AM74" t="s" s="2">
         <v>43</v>
@@ -10027,7 +10029,7 @@
     </row>
     <row r="75" hidden="true">
       <c r="A75" t="s" s="2">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" t="s" s="2">
@@ -10050,13 +10052,13 @@
         <v>53</v>
       </c>
       <c r="J75" t="s" s="2">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="K75" t="s" s="2">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="L75" t="s" s="2">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="M75" s="2"/>
       <c r="N75" s="2"/>
@@ -10107,7 +10109,7 @@
         <v>43</v>
       </c>
       <c r="AE75" t="s" s="2">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="AF75" t="s" s="2">
         <v>52</v>
@@ -10119,7 +10121,7 @@
         <v>43</v>
       </c>
       <c r="AI75" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ75" t="s" s="2">
         <v>43</v>
@@ -10128,7 +10130,7 @@
         <v>43</v>
       </c>
       <c r="AL75" t="s" s="2">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="AM75" t="s" s="2">
         <v>43</v>
@@ -10136,11 +10138,11 @@
     </row>
     <row r="76">
       <c r="A76" t="s" s="2">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" t="s" s="2">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="D76" s="2"/>
       <c r="E76" t="s" s="2">
@@ -10162,14 +10164,14 @@
         <v>54</v>
       </c>
       <c r="K76" t="s" s="2">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="L76" t="s" s="2">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="M76" s="2"/>
       <c r="N76" t="s" s="2">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="O76" t="s" s="2">
         <v>43</v>
@@ -10218,7 +10220,7 @@
         <v>43</v>
       </c>
       <c r="AE76" t="s" s="2">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="AF76" t="s" s="2">
         <v>41</v>
@@ -10230,16 +10232,16 @@
         <v>43</v>
       </c>
       <c r="AI76" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ76" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK76" t="s" s="2">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="AL76" t="s" s="2">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="AM76" t="s" s="2">
         <v>43</v>
@@ -10247,7 +10249,7 @@
     </row>
     <row r="77">
       <c r="A77" t="s" s="2">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" t="s" s="2">
@@ -10270,13 +10272,13 @@
         <v>43</v>
       </c>
       <c r="J77" t="s" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="K77" t="s" s="2">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="L77" t="s" s="2">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="M77" s="2"/>
       <c r="N77" s="2"/>
@@ -10303,13 +10305,13 @@
         <v>43</v>
       </c>
       <c r="W77" t="s" s="2">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="X77" t="s" s="2">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="Y77" t="s" s="2">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="Z77" t="s" s="2">
         <v>43</v>
@@ -10327,7 +10329,7 @@
         <v>43</v>
       </c>
       <c r="AE77" t="s" s="2">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="AF77" t="s" s="2">
         <v>41</v>
@@ -10339,16 +10341,16 @@
         <v>43</v>
       </c>
       <c r="AI77" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ77" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK77" t="s" s="2">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="AL77" t="s" s="2">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="AM77" t="s" s="2">
         <v>43</v>
@@ -10356,7 +10358,7 @@
     </row>
     <row r="78" hidden="true">
       <c r="A78" t="s" s="2">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" t="s" s="2">
@@ -10465,7 +10467,7 @@
     </row>
     <row r="79" hidden="true">
       <c r="A79" t="s" s="2">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" t="s" s="2">
@@ -10576,7 +10578,7 @@
     </row>
     <row r="80" hidden="true">
       <c r="A80" t="s" s="2">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" t="s" s="2">
@@ -10599,19 +10601,19 @@
         <v>53</v>
       </c>
       <c r="J80" t="s" s="2">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="K80" t="s" s="2">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="L80" t="s" s="2">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="M80" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="N80" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="O80" t="s" s="2">
         <v>43</v>
@@ -10648,7 +10650,7 @@
         <v>43</v>
       </c>
       <c r="AA80" t="s" s="2">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="AB80" s="2"/>
       <c r="AC80" t="s" s="2">
@@ -10658,7 +10660,7 @@
         <v>78</v>
       </c>
       <c r="AE80" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="AF80" t="s" s="2">
         <v>41</v>
@@ -10670,16 +10672,16 @@
         <v>43</v>
       </c>
       <c r="AI80" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ80" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK80" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="AL80" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="AM80" t="s" s="2">
         <v>43</v>
@@ -10687,10 +10689,10 @@
     </row>
     <row r="81" hidden="true">
       <c r="A81" t="s" s="2">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="B81" t="s" s="2">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="C81" t="s" s="2">
         <v>43</v>
@@ -10712,19 +10714,19 @@
         <v>53</v>
       </c>
       <c r="J81" t="s" s="2">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="K81" t="s" s="2">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="L81" t="s" s="2">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="M81" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="N81" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="O81" t="s" s="2">
         <v>43</v>
@@ -10749,13 +10751,13 @@
         <v>43</v>
       </c>
       <c r="W81" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="X81" t="s" s="2">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="Y81" t="s" s="2">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="Z81" t="s" s="2">
         <v>43</v>
@@ -10773,7 +10775,7 @@
         <v>43</v>
       </c>
       <c r="AE81" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="AF81" t="s" s="2">
         <v>41</v>
@@ -10785,16 +10787,16 @@
         <v>43</v>
       </c>
       <c r="AI81" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ81" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK81" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="AL81" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="AM81" t="s" s="2">
         <v>43</v>
@@ -10802,7 +10804,7 @@
     </row>
     <row r="82" hidden="true">
       <c r="A82" t="s" s="2">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="B82" s="2"/>
       <c r="C82" t="s" s="2">
@@ -10828,16 +10830,16 @@
         <v>54</v>
       </c>
       <c r="K82" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="L82" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="M82" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="N82" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="O82" t="s" s="2">
         <v>43</v>
@@ -10886,7 +10888,7 @@
         <v>43</v>
       </c>
       <c r="AE82" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AF82" t="s" s="2">
         <v>41</v>
@@ -10898,16 +10900,16 @@
         <v>43</v>
       </c>
       <c r="AI82" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ82" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK82" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AL82" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AM82" t="s" s="2">
         <v>43</v>
@@ -10915,7 +10917,7 @@
     </row>
     <row r="83">
       <c r="A83" t="s" s="2">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="B83" s="2"/>
       <c r="C83" t="s" s="2">
@@ -10938,19 +10940,19 @@
         <v>43</v>
       </c>
       <c r="J83" t="s" s="2">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="K83" t="s" s="2">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="L83" t="s" s="2">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="M83" t="s" s="2">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="N83" t="s" s="2">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="O83" t="s" s="2">
         <v>43</v>
@@ -10999,7 +11001,7 @@
         <v>43</v>
       </c>
       <c r="AE83" t="s" s="2">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="AF83" t="s" s="2">
         <v>41</v>
@@ -11011,16 +11013,16 @@
         <v>43</v>
       </c>
       <c r="AI83" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ83" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK83" t="s" s="2">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="AL83" t="s" s="2">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="AM83" t="s" s="2">
         <v>43</v>

</xml_diff>

<commit_message>
Fixed category (pattern) issue in Diagnostic Report IG
Closes #87
</commit_message>
<xml_diff>
--- a/output/DiagnosticReport/diagnosticreport-imag-atomic-1.xlsx
+++ b/output/DiagnosticReport/diagnosticreport-imag-atomic-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2918" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2918" uniqueCount="502">
   <si>
     <t>Path</t>
   </si>
@@ -160,7 +160,7 @@
   </si>
   <si>
     <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}inv-dh-dir-01:The subject shall at least have a reference or an identifier with at least a system and a value {subject.reference.exists() or subject.identifier.where(system.count() + value.count() &gt;1).exists()}inv-dh-dir-02:The performer shall at least have a reference or an identifier with at least a system and a value {performer.reference.exists() or performer.identifier.where(system.count() + value.count() &gt;1).exists()}</t>
+dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}inv-dh-dir-04:One category shall be 'imaging' 'http://terminology.hl7.org/CodeSystem/observation-category' {category.coding.where(system='http://terminology.hl7.org/CodeSystem/observation-category' and code='imaging').exists()}inv-dh-dir-01:The subject shall at least have a reference or an identifier with at least a system and a value {subject.reference.exists() or subject.identifier.where(system.count() + value.count() &gt;1).exists()}inv-dh-dir-02:The performer shall at least have a reference or an identifier with at least a system and a value {performer.reference.exists() or performer.identifier.where(system.count() + value.count() &gt;1).exists()}</t>
   </si>
   <si>
     <t>Event</t>
@@ -1072,14 +1072,6 @@
   </si>
   <si>
     <t>Multiple categories are allowed using various categorization schemes.   The level of granularity is defined by the category concepts in the value set. More fine-grained filtering can be performed using the metadata and/or terminology hierarchy in DiagnosticReport.code.</t>
-  </si>
-  <si>
-    <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
-  &lt;coding&gt;
-    &lt;system value="http://terminology.hl7.org/CodeSystem/observation-category"/&gt;
-    &lt;code value="imaging"/&gt;
-  &lt;/coding&gt;
-&lt;/valueCodeableConcept&gt;</t>
   </si>
   <si>
     <t>http://hl7.org/fhir/ValueSet/diagnostic-service-sections</t>
@@ -7063,7 +7055,7 @@
         <v>43</v>
       </c>
       <c r="R48" t="s" s="2">
-        <v>340</v>
+        <v>43</v>
       </c>
       <c r="S48" t="s" s="2">
         <v>43</v>
@@ -7082,7 +7074,7 @@
       </c>
       <c r="X48" s="2"/>
       <c r="Y48" t="s" s="2">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="Z48" t="s" s="2">
         <v>43</v>
@@ -7118,22 +7110,22 @@
         <v>43</v>
       </c>
       <c r="AK48" t="s" s="2">
+        <v>341</v>
+      </c>
+      <c r="AL48" t="s" s="2">
         <v>342</v>
       </c>
-      <c r="AL48" t="s" s="2">
+      <c r="AM48" t="s" s="2">
         <v>343</v>
-      </c>
-      <c r="AM48" t="s" s="2">
-        <v>344</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="2">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" t="s" s="2">
@@ -7155,10 +7147,10 @@
         <v>190</v>
       </c>
       <c r="K49" t="s" s="2">
+        <v>346</v>
+      </c>
+      <c r="L49" t="s" s="2">
         <v>347</v>
-      </c>
-      <c r="L49" t="s" s="2">
-        <v>348</v>
       </c>
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
@@ -7188,11 +7180,11 @@
         <v>134</v>
       </c>
       <c r="X49" t="s" s="2">
+        <v>348</v>
+      </c>
+      <c r="Y49" t="s" s="2">
         <v>349</v>
       </c>
-      <c r="Y49" t="s" s="2">
-        <v>350</v>
-      </c>
       <c r="Z49" t="s" s="2">
         <v>43</v>
       </c>
@@ -7209,7 +7201,7 @@
         <v>43</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>52</v>
@@ -7224,21 +7216,21 @@
         <v>87</v>
       </c>
       <c r="AJ49" t="s" s="2">
+        <v>350</v>
+      </c>
+      <c r="AK49" t="s" s="2">
         <v>351</v>
       </c>
-      <c r="AK49" t="s" s="2">
+      <c r="AL49" t="s" s="2">
         <v>352</v>
       </c>
-      <c r="AL49" t="s" s="2">
+      <c r="AM49" t="s" s="2">
         <v>353</v>
-      </c>
-      <c r="AM49" t="s" s="2">
-        <v>354</v>
       </c>
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -7347,7 +7339,7 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -7458,7 +7450,7 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -7530,7 +7522,7 @@
         <v>43</v>
       </c>
       <c r="AA52" t="s" s="2">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="AB52" s="2"/>
       <c r="AC52" t="s" s="2">
@@ -7569,10 +7561,10 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B53" t="s" s="2">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C53" t="s" s="2">
         <v>43</v>
@@ -7597,7 +7589,7 @@
         <v>107</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="L53" t="s" s="2">
         <v>202</v>
@@ -7635,7 +7627,7 @@
       </c>
       <c r="X53" s="2"/>
       <c r="Y53" t="s" s="2">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="Z53" t="s" s="2">
         <v>43</v>
@@ -7682,7 +7674,7 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -7795,11 +7787,11 @@
     </row>
     <row r="55">
       <c r="A55" t="s" s="2">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" t="s" s="2">
@@ -7818,17 +7810,17 @@
         <v>53</v>
       </c>
       <c r="J55" t="s" s="2">
+        <v>364</v>
+      </c>
+      <c r="K55" t="s" s="2">
         <v>365</v>
       </c>
-      <c r="K55" t="s" s="2">
+      <c r="L55" t="s" s="2">
         <v>366</v>
-      </c>
-      <c r="L55" t="s" s="2">
-        <v>367</v>
       </c>
       <c r="M55" s="2"/>
       <c r="N55" t="s" s="2">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="O55" t="s" s="2">
         <v>43</v>
@@ -7877,7 +7869,7 @@
         <v>43</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>41</v>
@@ -7892,25 +7884,25 @@
         <v>87</v>
       </c>
       <c r="AJ55" t="s" s="2">
+        <v>368</v>
+      </c>
+      <c r="AK55" t="s" s="2">
         <v>369</v>
       </c>
-      <c r="AK55" t="s" s="2">
+      <c r="AL55" t="s" s="2">
         <v>370</v>
       </c>
-      <c r="AL55" t="s" s="2">
+      <c r="AM55" t="s" s="2">
         <v>371</v>
-      </c>
-      <c r="AM55" t="s" s="2">
-        <v>372</v>
       </c>
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" t="s" s="2">
@@ -7929,19 +7921,19 @@
         <v>53</v>
       </c>
       <c r="J56" t="s" s="2">
+        <v>374</v>
+      </c>
+      <c r="K56" t="s" s="2">
         <v>375</v>
       </c>
-      <c r="K56" t="s" s="2">
+      <c r="L56" t="s" s="2">
         <v>376</v>
       </c>
-      <c r="L56" t="s" s="2">
+      <c r="M56" t="s" s="2">
         <v>377</v>
       </c>
-      <c r="M56" t="s" s="2">
+      <c r="N56" t="s" s="2">
         <v>378</v>
-      </c>
-      <c r="N56" t="s" s="2">
-        <v>379</v>
       </c>
       <c r="O56" t="s" s="2">
         <v>43</v>
@@ -7990,7 +7982,7 @@
         <v>43</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>41</v>
@@ -8005,25 +7997,25 @@
         <v>87</v>
       </c>
       <c r="AJ56" t="s" s="2">
+        <v>379</v>
+      </c>
+      <c r="AK56" t="s" s="2">
         <v>380</v>
       </c>
-      <c r="AK56" t="s" s="2">
+      <c r="AL56" t="s" s="2">
         <v>381</v>
       </c>
-      <c r="AL56" t="s" s="2">
+      <c r="AM56" t="s" s="2">
         <v>382</v>
-      </c>
-      <c r="AM56" t="s" s="2">
-        <v>383</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="2">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" t="s" s="2">
@@ -8042,19 +8034,19 @@
         <v>53</v>
       </c>
       <c r="J57" t="s" s="2">
+        <v>385</v>
+      </c>
+      <c r="K57" t="s" s="2">
         <v>386</v>
       </c>
-      <c r="K57" t="s" s="2">
+      <c r="L57" t="s" s="2">
         <v>387</v>
       </c>
-      <c r="L57" t="s" s="2">
+      <c r="M57" t="s" s="2">
         <v>388</v>
       </c>
-      <c r="M57" t="s" s="2">
+      <c r="N57" t="s" s="2">
         <v>389</v>
-      </c>
-      <c r="N57" t="s" s="2">
-        <v>390</v>
       </c>
       <c r="O57" t="s" s="2">
         <v>43</v>
@@ -8103,7 +8095,7 @@
         <v>43</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>41</v>
@@ -8118,25 +8110,25 @@
         <v>87</v>
       </c>
       <c r="AJ57" t="s" s="2">
+        <v>390</v>
+      </c>
+      <c r="AK57" t="s" s="2">
         <v>391</v>
       </c>
-      <c r="AK57" t="s" s="2">
+      <c r="AL57" t="s" s="2">
         <v>392</v>
       </c>
-      <c r="AL57" t="s" s="2">
+      <c r="AM57" t="s" s="2">
         <v>393</v>
-      </c>
-      <c r="AM57" t="s" s="2">
-        <v>394</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="2">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" t="s" s="2">
@@ -8158,16 +8150,16 @@
         <v>89</v>
       </c>
       <c r="K58" t="s" s="2">
+        <v>396</v>
+      </c>
+      <c r="L58" t="s" s="2">
         <v>397</v>
       </c>
-      <c r="L58" t="s" s="2">
+      <c r="M58" t="s" s="2">
         <v>398</v>
       </c>
-      <c r="M58" t="s" s="2">
+      <c r="N58" t="s" s="2">
         <v>399</v>
-      </c>
-      <c r="N58" t="s" s="2">
-        <v>400</v>
       </c>
       <c r="O58" t="s" s="2">
         <v>43</v>
@@ -8216,7 +8208,7 @@
         <v>43</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>41</v>
@@ -8234,22 +8226,22 @@
         <v>43</v>
       </c>
       <c r="AK58" t="s" s="2">
+        <v>400</v>
+      </c>
+      <c r="AL58" t="s" s="2">
         <v>401</v>
       </c>
-      <c r="AL58" t="s" s="2">
+      <c r="AM58" t="s" s="2">
         <v>402</v>
-      </c>
-      <c r="AM58" t="s" s="2">
-        <v>403</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="2">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" t="s" s="2">
@@ -8268,19 +8260,19 @@
         <v>53</v>
       </c>
       <c r="J59" t="s" s="2">
+        <v>405</v>
+      </c>
+      <c r="K59" t="s" s="2">
         <v>406</v>
       </c>
-      <c r="K59" t="s" s="2">
+      <c r="L59" t="s" s="2">
         <v>407</v>
       </c>
-      <c r="L59" t="s" s="2">
+      <c r="M59" t="s" s="2">
         <v>408</v>
       </c>
-      <c r="M59" t="s" s="2">
+      <c r="N59" t="s" s="2">
         <v>409</v>
-      </c>
-      <c r="N59" t="s" s="2">
-        <v>410</v>
       </c>
       <c r="O59" t="s" s="2">
         <v>43</v>
@@ -8329,7 +8321,7 @@
         <v>43</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>41</v>
@@ -8344,25 +8336,25 @@
         <v>87</v>
       </c>
       <c r="AJ59" t="s" s="2">
+        <v>410</v>
+      </c>
+      <c r="AK59" t="s" s="2">
         <v>411</v>
       </c>
-      <c r="AK59" t="s" s="2">
+      <c r="AL59" t="s" s="2">
         <v>412</v>
       </c>
-      <c r="AL59" t="s" s="2">
+      <c r="AM59" t="s" s="2">
         <v>413</v>
-      </c>
-      <c r="AM59" t="s" s="2">
-        <v>414</v>
       </c>
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" t="s" s="2">
@@ -8381,19 +8373,19 @@
         <v>53</v>
       </c>
       <c r="J60" t="s" s="2">
+        <v>416</v>
+      </c>
+      <c r="K60" t="s" s="2">
         <v>417</v>
       </c>
-      <c r="K60" t="s" s="2">
+      <c r="L60" t="s" s="2">
         <v>418</v>
       </c>
-      <c r="L60" t="s" s="2">
+      <c r="M60" t="s" s="2">
         <v>419</v>
       </c>
-      <c r="M60" t="s" s="2">
-        <v>420</v>
-      </c>
       <c r="N60" t="s" s="2">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="O60" t="s" s="2">
         <v>43</v>
@@ -8442,7 +8434,7 @@
         <v>43</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>41</v>
@@ -8457,21 +8449,21 @@
         <v>87</v>
       </c>
       <c r="AJ60" t="s" s="2">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="AK60" t="s" s="2">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AL60" t="s" s="2">
+        <v>412</v>
+      </c>
+      <c r="AM60" t="s" s="2">
         <v>413</v>
-      </c>
-      <c r="AM60" t="s" s="2">
-        <v>414</v>
       </c>
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
@@ -8494,19 +8486,19 @@
         <v>43</v>
       </c>
       <c r="J61" t="s" s="2">
+        <v>422</v>
+      </c>
+      <c r="K61" t="s" s="2">
         <v>423</v>
       </c>
-      <c r="K61" t="s" s="2">
+      <c r="L61" t="s" s="2">
         <v>424</v>
       </c>
-      <c r="L61" t="s" s="2">
+      <c r="M61" t="s" s="2">
         <v>425</v>
       </c>
-      <c r="M61" t="s" s="2">
+      <c r="N61" t="s" s="2">
         <v>426</v>
-      </c>
-      <c r="N61" t="s" s="2">
-        <v>427</v>
       </c>
       <c r="O61" t="s" s="2">
         <v>43</v>
@@ -8555,7 +8547,7 @@
         <v>43</v>
       </c>
       <c r="AE61" t="s" s="2">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="AF61" t="s" s="2">
         <v>41</v>
@@ -8573,10 +8565,10 @@
         <v>43</v>
       </c>
       <c r="AK61" t="s" s="2">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="AL61" t="s" s="2">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="AM61" t="s" s="2">
         <v>43</v>
@@ -8584,11 +8576,11 @@
     </row>
     <row r="62">
       <c r="A62" t="s" s="2">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" t="s" s="2">
@@ -8607,19 +8599,19 @@
         <v>43</v>
       </c>
       <c r="J62" t="s" s="2">
+        <v>430</v>
+      </c>
+      <c r="K62" t="s" s="2">
         <v>431</v>
       </c>
-      <c r="K62" t="s" s="2">
+      <c r="L62" t="s" s="2">
         <v>432</v>
       </c>
-      <c r="L62" t="s" s="2">
+      <c r="M62" t="s" s="2">
         <v>433</v>
       </c>
-      <c r="M62" t="s" s="2">
+      <c r="N62" t="s" s="2">
         <v>434</v>
-      </c>
-      <c r="N62" t="s" s="2">
-        <v>435</v>
       </c>
       <c r="O62" t="s" s="2">
         <v>43</v>
@@ -8668,7 +8660,7 @@
         <v>43</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>41</v>
@@ -8686,10 +8678,10 @@
         <v>43</v>
       </c>
       <c r="AK62" t="s" s="2">
+        <v>435</v>
+      </c>
+      <c r="AL62" t="s" s="2">
         <v>436</v>
-      </c>
-      <c r="AL62" t="s" s="2">
-        <v>437</v>
       </c>
       <c r="AM62" t="s" s="2">
         <v>43</v>
@@ -8697,7 +8689,7 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
@@ -8806,7 +8798,7 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
@@ -8917,7 +8909,7 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
@@ -9028,7 +9020,7 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
@@ -9139,7 +9131,7 @@
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" t="s" s="2">
@@ -9250,7 +9242,7 @@
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" t="s" s="2">
@@ -9361,7 +9353,7 @@
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" t="s" s="2">
@@ -9384,16 +9376,16 @@
         <v>43</v>
       </c>
       <c r="J69" t="s" s="2">
+        <v>444</v>
+      </c>
+      <c r="K69" t="s" s="2">
         <v>445</v>
       </c>
-      <c r="K69" t="s" s="2">
+      <c r="L69" t="s" s="2">
         <v>446</v>
       </c>
-      <c r="L69" t="s" s="2">
+      <c r="M69" t="s" s="2">
         <v>447</v>
-      </c>
-      <c r="M69" t="s" s="2">
-        <v>448</v>
       </c>
       <c r="N69" s="2"/>
       <c r="O69" t="s" s="2">
@@ -9443,7 +9435,7 @@
         <v>43</v>
       </c>
       <c r="AE69" t="s" s="2">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="AF69" t="s" s="2">
         <v>41</v>
@@ -9464,7 +9456,7 @@
         <v>43</v>
       </c>
       <c r="AL69" t="s" s="2">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="AM69" t="s" s="2">
         <v>43</v>
@@ -9472,11 +9464,11 @@
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" t="s" s="2">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D70" s="2"/>
       <c r="E70" t="s" s="2">
@@ -9495,17 +9487,17 @@
         <v>53</v>
       </c>
       <c r="J70" t="s" s="2">
+        <v>451</v>
+      </c>
+      <c r="K70" t="s" s="2">
         <v>452</v>
       </c>
-      <c r="K70" t="s" s="2">
+      <c r="L70" t="s" s="2">
         <v>453</v>
-      </c>
-      <c r="L70" t="s" s="2">
-        <v>454</v>
       </c>
       <c r="M70" s="2"/>
       <c r="N70" t="s" s="2">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="O70" t="s" s="2">
         <v>43</v>
@@ -9554,7 +9546,7 @@
         <v>43</v>
       </c>
       <c r="AE70" t="s" s="2">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="AF70" t="s" s="2">
         <v>41</v>
@@ -9572,10 +9564,10 @@
         <v>43</v>
       </c>
       <c r="AK70" t="s" s="2">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="AL70" t="s" s="2">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="AM70" t="s" s="2">
         <v>43</v>
@@ -9583,7 +9575,7 @@
     </row>
     <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" t="s" s="2">
@@ -9692,7 +9684,7 @@
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" t="s" s="2">
@@ -9803,11 +9795,11 @@
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" t="s" s="2">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D73" s="2"/>
       <c r="E73" t="s" s="2">
@@ -9829,10 +9821,10 @@
         <v>72</v>
       </c>
       <c r="K73" t="s" s="2">
+        <v>460</v>
+      </c>
+      <c r="L73" t="s" s="2">
         <v>461</v>
-      </c>
-      <c r="L73" t="s" s="2">
-        <v>462</v>
       </c>
       <c r="M73" t="s" s="2">
         <v>75</v>
@@ -9887,7 +9879,7 @@
         <v>43</v>
       </c>
       <c r="AE73" t="s" s="2">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="AF73" t="s" s="2">
         <v>41</v>
@@ -9916,7 +9908,7 @@
     </row>
     <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" t="s" s="2">
@@ -9942,16 +9934,16 @@
         <v>54</v>
       </c>
       <c r="K74" t="s" s="2">
+        <v>464</v>
+      </c>
+      <c r="L74" t="s" s="2">
         <v>465</v>
       </c>
-      <c r="L74" t="s" s="2">
+      <c r="M74" t="s" s="2">
         <v>466</v>
       </c>
-      <c r="M74" t="s" s="2">
+      <c r="N74" t="s" s="2">
         <v>467</v>
-      </c>
-      <c r="N74" t="s" s="2">
-        <v>468</v>
       </c>
       <c r="O74" t="s" s="2">
         <v>43</v>
@@ -10000,7 +9992,7 @@
         <v>43</v>
       </c>
       <c r="AE74" t="s" s="2">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="AF74" t="s" s="2">
         <v>41</v>
@@ -10021,7 +10013,7 @@
         <v>43</v>
       </c>
       <c r="AL74" t="s" s="2">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="AM74" t="s" s="2">
         <v>43</v>
@@ -10029,7 +10021,7 @@
     </row>
     <row r="75" hidden="true">
       <c r="A75" t="s" s="2">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" t="s" s="2">
@@ -10052,13 +10044,13 @@
         <v>53</v>
       </c>
       <c r="J75" t="s" s="2">
+        <v>470</v>
+      </c>
+      <c r="K75" t="s" s="2">
         <v>471</v>
       </c>
-      <c r="K75" t="s" s="2">
+      <c r="L75" t="s" s="2">
         <v>472</v>
-      </c>
-      <c r="L75" t="s" s="2">
-        <v>473</v>
       </c>
       <c r="M75" s="2"/>
       <c r="N75" s="2"/>
@@ -10109,7 +10101,7 @@
         <v>43</v>
       </c>
       <c r="AE75" t="s" s="2">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="AF75" t="s" s="2">
         <v>52</v>
@@ -10130,7 +10122,7 @@
         <v>43</v>
       </c>
       <c r="AL75" t="s" s="2">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="AM75" t="s" s="2">
         <v>43</v>
@@ -10138,11 +10130,11 @@
     </row>
     <row r="76">
       <c r="A76" t="s" s="2">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" t="s" s="2">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D76" s="2"/>
       <c r="E76" t="s" s="2">
@@ -10164,14 +10156,14 @@
         <v>54</v>
       </c>
       <c r="K76" t="s" s="2">
+        <v>476</v>
+      </c>
+      <c r="L76" t="s" s="2">
         <v>477</v>
-      </c>
-      <c r="L76" t="s" s="2">
-        <v>478</v>
       </c>
       <c r="M76" s="2"/>
       <c r="N76" t="s" s="2">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="O76" t="s" s="2">
         <v>43</v>
@@ -10220,7 +10212,7 @@
         <v>43</v>
       </c>
       <c r="AE76" t="s" s="2">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="AF76" t="s" s="2">
         <v>41</v>
@@ -10238,10 +10230,10 @@
         <v>43</v>
       </c>
       <c r="AK76" t="s" s="2">
+        <v>479</v>
+      </c>
+      <c r="AL76" t="s" s="2">
         <v>480</v>
-      </c>
-      <c r="AL76" t="s" s="2">
-        <v>481</v>
       </c>
       <c r="AM76" t="s" s="2">
         <v>43</v>
@@ -10249,7 +10241,7 @@
     </row>
     <row r="77">
       <c r="A77" t="s" s="2">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" t="s" s="2">
@@ -10275,10 +10267,10 @@
         <v>190</v>
       </c>
       <c r="K77" t="s" s="2">
+        <v>482</v>
+      </c>
+      <c r="L77" t="s" s="2">
         <v>483</v>
-      </c>
-      <c r="L77" t="s" s="2">
-        <v>484</v>
       </c>
       <c r="M77" s="2"/>
       <c r="N77" s="2"/>
@@ -10308,11 +10300,11 @@
         <v>119</v>
       </c>
       <c r="X77" t="s" s="2">
+        <v>484</v>
+      </c>
+      <c r="Y77" t="s" s="2">
         <v>485</v>
       </c>
-      <c r="Y77" t="s" s="2">
-        <v>486</v>
-      </c>
       <c r="Z77" t="s" s="2">
         <v>43</v>
       </c>
@@ -10329,7 +10321,7 @@
         <v>43</v>
       </c>
       <c r="AE77" t="s" s="2">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="AF77" t="s" s="2">
         <v>41</v>
@@ -10347,10 +10339,10 @@
         <v>43</v>
       </c>
       <c r="AK77" t="s" s="2">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="AL77" t="s" s="2">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="AM77" t="s" s="2">
         <v>43</v>
@@ -10358,7 +10350,7 @@
     </row>
     <row r="78" hidden="true">
       <c r="A78" t="s" s="2">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" t="s" s="2">
@@ -10467,7 +10459,7 @@
     </row>
     <row r="79" hidden="true">
       <c r="A79" t="s" s="2">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" t="s" s="2">
@@ -10578,7 +10570,7 @@
     </row>
     <row r="80" hidden="true">
       <c r="A80" t="s" s="2">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" t="s" s="2">
@@ -10650,7 +10642,7 @@
         <v>43</v>
       </c>
       <c r="AA80" t="s" s="2">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="AB80" s="2"/>
       <c r="AC80" t="s" s="2">
@@ -10689,10 +10681,10 @@
     </row>
     <row r="81" hidden="true">
       <c r="A81" t="s" s="2">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B81" t="s" s="2">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C81" t="s" s="2">
         <v>43</v>
@@ -10717,7 +10709,7 @@
         <v>107</v>
       </c>
       <c r="K81" t="s" s="2">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="L81" t="s" s="2">
         <v>202</v>
@@ -10754,10 +10746,10 @@
         <v>184</v>
       </c>
       <c r="X81" t="s" s="2">
+        <v>492</v>
+      </c>
+      <c r="Y81" t="s" s="2">
         <v>493</v>
-      </c>
-      <c r="Y81" t="s" s="2">
-        <v>494</v>
       </c>
       <c r="Z81" t="s" s="2">
         <v>43</v>
@@ -10804,7 +10796,7 @@
     </row>
     <row r="82" hidden="true">
       <c r="A82" t="s" s="2">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B82" s="2"/>
       <c r="C82" t="s" s="2">
@@ -10917,7 +10909,7 @@
     </row>
     <row r="83">
       <c r="A83" t="s" s="2">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B83" s="2"/>
       <c r="C83" t="s" s="2">
@@ -10940,19 +10932,19 @@
         <v>43</v>
       </c>
       <c r="J83" t="s" s="2">
+        <v>496</v>
+      </c>
+      <c r="K83" t="s" s="2">
         <v>497</v>
       </c>
-      <c r="K83" t="s" s="2">
+      <c r="L83" t="s" s="2">
         <v>498</v>
       </c>
-      <c r="L83" t="s" s="2">
+      <c r="M83" t="s" s="2">
         <v>499</v>
       </c>
-      <c r="M83" t="s" s="2">
+      <c r="N83" t="s" s="2">
         <v>500</v>
-      </c>
-      <c r="N83" t="s" s="2">
-        <v>501</v>
       </c>
       <c r="O83" t="s" s="2">
         <v>43</v>
@@ -11001,7 +10993,7 @@
         <v>43</v>
       </c>
       <c r="AE83" t="s" s="2">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="AF83" t="s" s="2">
         <v>41</v>
@@ -11019,10 +11011,10 @@
         <v>43</v>
       </c>
       <c r="AK83" t="s" s="2">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="AL83" t="s" s="2">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="AM83" t="s" s="2">
         <v>43</v>

</xml_diff>

<commit_message>
Remove references to snomed imaging procedures slice of code.
</commit_message>
<xml_diff>
--- a/output/DiagnosticReport/diagnosticreport-imag-atomic-1.xlsx
+++ b/output/DiagnosticReport/diagnosticreport-imag-atomic-1.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AM$83</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AM$73</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2918" uniqueCount="502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2564" uniqueCount="485">
   <si>
     <t>Path</t>
   </si>
@@ -1117,31 +1117,6 @@
     <t>FiveWs.what[x]</t>
   </si>
   <si>
-    <t>DiagnosticReport.code.id</t>
-  </si>
-  <si>
-    <t>DiagnosticReport.code.extension</t>
-  </si>
-  <si>
-    <t>DiagnosticReport.code.coding</t>
-  </si>
-  <si>
-    <t>value:system}
-value:code}</t>
-  </si>
-  <si>
-    <t>snomedImagingProcedures</t>
-  </si>
-  <si>
-    <t>Diagnostic Imaging Procedures (SNOMED CT)</t>
-  </si>
-  <si>
-    <t>https://healthterminologies.gov.au/fhir/ValueSet/imaging-procedure-1</t>
-  </si>
-  <si>
-    <t>DiagnosticReport.code.text</t>
-  </si>
-  <si>
     <t>DiagnosticReport.subject</t>
   </si>
   <si>
@@ -1529,38 +1504,10 @@
     <t>One or more codes that represent the summary conclusion (interpretation/impression) of the diagnostic report.</t>
   </si>
   <si>
-    <t>Diagnosis codes provided as adjuncts to the report.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/clinical-findings</t>
+    <t>https://healthterminologies.gov.au/fhir/ValueSet/clinical-finding-1</t>
   </si>
   <si>
     <t>inboundRelationship[typeCode=SPRT].source[classCode=OBS, moodCode=EVN, code=LOINC:54531-9].value (type=CD)</t>
-  </si>
-  <si>
-    <t>DiagnosticReport.conclusionCode.id</t>
-  </si>
-  <si>
-    <t>DiagnosticReport.conclusionCode.extension</t>
-  </si>
-  <si>
-    <t>DiagnosticReport.conclusionCode.coding</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value:system}
-</t>
-  </si>
-  <si>
-    <t>snomedFinding</t>
-  </si>
-  <si>
-    <t>Clinical Finding (SNOMED CT)</t>
-  </si>
-  <si>
-    <t>https://healthterminologies.gov.au/fhir/ValueSet/clinical-finding-1</t>
-  </si>
-  <si>
-    <t>DiagnosticReport.conclusionCode.text</t>
   </si>
   <si>
     <t>DiagnosticReport.presentedForm</t>
@@ -1731,7 +1678,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AM83"/>
+  <dimension ref="A1:AM73"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1741,7 +1688,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="48.28125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="25.44140625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="13.32421875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="60.54296875" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>
@@ -7228,41 +7175,43 @@
         <v>353</v>
       </c>
     </row>
-    <row r="50" hidden="true">
+    <row r="50">
       <c r="A50" t="s" s="2">
         <v>354</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
-        <v>43</v>
+        <v>355</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" t="s" s="2">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="F50" t="s" s="2">
         <v>52</v>
       </c>
       <c r="G50" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="H50" t="s" s="2">
         <v>43</v>
       </c>
       <c r="I50" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>54</v>
+        <v>356</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>66</v>
+        <v>357</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>67</v>
+        <v>358</v>
       </c>
       <c r="M50" s="2"/>
-      <c r="N50" s="2"/>
+      <c r="N50" t="s" s="2">
+        <v>359</v>
+      </c>
       <c r="O50" t="s" s="2">
         <v>43</v>
       </c>
@@ -7310,7 +7259,7 @@
         <v>43</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>68</v>
+        <v>354</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>41</v>
@@ -7322,35 +7271,35 @@
         <v>43</v>
       </c>
       <c r="AI50" t="s" s="2">
-        <v>43</v>
+        <v>87</v>
       </c>
       <c r="AJ50" t="s" s="2">
-        <v>43</v>
+        <v>360</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>43</v>
+        <v>361</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>69</v>
+        <v>362</v>
       </c>
       <c r="AM50" t="s" s="2">
-        <v>43</v>
+        <v>363</v>
       </c>
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>355</v>
+        <v>364</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
-        <v>71</v>
+        <v>365</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F51" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="G51" t="s" s="2">
         <v>43</v>
@@ -7359,21 +7308,23 @@
         <v>43</v>
       </c>
       <c r="I51" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>72</v>
+        <v>366</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>73</v>
+        <v>367</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>74</v>
+        <v>368</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="N51" s="2"/>
+        <v>369</v>
+      </c>
+      <c r="N51" t="s" s="2">
+        <v>370</v>
+      </c>
       <c r="O51" t="s" s="2">
         <v>43</v>
       </c>
@@ -7409,62 +7360,62 @@
         <v>43</v>
       </c>
       <c r="AA51" t="s" s="2">
-        <v>76</v>
+        <v>43</v>
       </c>
       <c r="AB51" t="s" s="2">
-        <v>77</v>
+        <v>43</v>
       </c>
       <c r="AC51" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AD51" t="s" s="2">
-        <v>78</v>
+        <v>43</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>79</v>
+        <v>364</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG51" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="AH51" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AI51" t="s" s="2">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="AJ51" t="s" s="2">
-        <v>43</v>
+        <v>371</v>
       </c>
       <c r="AK51" t="s" s="2">
-        <v>43</v>
+        <v>372</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>69</v>
+        <v>373</v>
       </c>
       <c r="AM51" t="s" s="2">
-        <v>43</v>
+        <v>374</v>
       </c>
     </row>
-    <row r="52" hidden="true">
+    <row r="52">
       <c r="A52" t="s" s="2">
-        <v>356</v>
+        <v>375</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
-        <v>43</v>
+        <v>376</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" t="s" s="2">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="F52" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="G52" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="H52" t="s" s="2">
         <v>43</v>
@@ -7473,19 +7424,19 @@
         <v>53</v>
       </c>
       <c r="J52" t="s" s="2">
-        <v>107</v>
+        <v>377</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>201</v>
+        <v>378</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>202</v>
+        <v>379</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>203</v>
+        <v>380</v>
       </c>
       <c r="N52" t="s" s="2">
-        <v>204</v>
+        <v>381</v>
       </c>
       <c r="O52" t="s" s="2">
         <v>43</v>
@@ -7522,23 +7473,25 @@
         <v>43</v>
       </c>
       <c r="AA52" t="s" s="2">
-        <v>357</v>
-      </c>
-      <c r="AB52" s="2"/>
+        <v>43</v>
+      </c>
+      <c r="AB52" t="s" s="2">
+        <v>43</v>
+      </c>
       <c r="AC52" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AD52" t="s" s="2">
-        <v>78</v>
+        <v>43</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>205</v>
+        <v>375</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG52" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="AH52" t="s" s="2">
         <v>43</v>
@@ -7547,27 +7500,25 @@
         <v>87</v>
       </c>
       <c r="AJ52" t="s" s="2">
-        <v>43</v>
+        <v>382</v>
       </c>
       <c r="AK52" t="s" s="2">
-        <v>206</v>
+        <v>383</v>
       </c>
       <c r="AL52" t="s" s="2">
-        <v>207</v>
+        <v>384</v>
       </c>
       <c r="AM52" t="s" s="2">
-        <v>43</v>
+        <v>385</v>
       </c>
     </row>
-    <row r="53" hidden="true">
+    <row r="53">
       <c r="A53" t="s" s="2">
-        <v>356</v>
-      </c>
-      <c r="B53" t="s" s="2">
-        <v>358</v>
-      </c>
+        <v>386</v>
+      </c>
+      <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
-        <v>43</v>
+        <v>387</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" t="s" s="2">
@@ -7577,7 +7528,7 @@
         <v>52</v>
       </c>
       <c r="G53" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="H53" t="s" s="2">
         <v>43</v>
@@ -7586,19 +7537,19 @@
         <v>53</v>
       </c>
       <c r="J53" t="s" s="2">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>359</v>
+        <v>388</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>202</v>
+        <v>389</v>
       </c>
       <c r="M53" t="s" s="2">
-        <v>203</v>
+        <v>390</v>
       </c>
       <c r="N53" t="s" s="2">
-        <v>204</v>
+        <v>391</v>
       </c>
       <c r="O53" t="s" s="2">
         <v>43</v>
@@ -7623,11 +7574,13 @@
         <v>43</v>
       </c>
       <c r="W53" t="s" s="2">
-        <v>184</v>
-      </c>
-      <c r="X53" s="2"/>
+        <v>43</v>
+      </c>
+      <c r="X53" t="s" s="2">
+        <v>43</v>
+      </c>
       <c r="Y53" t="s" s="2">
-        <v>360</v>
+        <v>43</v>
       </c>
       <c r="Z53" t="s" s="2">
         <v>43</v>
@@ -7645,13 +7598,13 @@
         <v>43</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>205</v>
+        <v>386</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG53" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="AH53" t="s" s="2">
         <v>43</v>
@@ -7663,32 +7616,32 @@
         <v>43</v>
       </c>
       <c r="AK53" t="s" s="2">
-        <v>206</v>
+        <v>392</v>
       </c>
       <c r="AL53" t="s" s="2">
-        <v>207</v>
+        <v>393</v>
       </c>
       <c r="AM53" t="s" s="2">
-        <v>43</v>
+        <v>394</v>
       </c>
     </row>
-    <row r="54" hidden="true">
+    <row r="54">
       <c r="A54" t="s" s="2">
-        <v>361</v>
+        <v>395</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
-        <v>43</v>
+        <v>396</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" t="s" s="2">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="F54" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G54" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="H54" t="s" s="2">
         <v>43</v>
@@ -7697,19 +7650,19 @@
         <v>53</v>
       </c>
       <c r="J54" t="s" s="2">
-        <v>54</v>
+        <v>397</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>251</v>
+        <v>398</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>252</v>
+        <v>399</v>
       </c>
       <c r="M54" t="s" s="2">
-        <v>253</v>
+        <v>400</v>
       </c>
       <c r="N54" t="s" s="2">
-        <v>254</v>
+        <v>401</v>
       </c>
       <c r="O54" t="s" s="2">
         <v>43</v>
@@ -7758,13 +7711,13 @@
         <v>43</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>255</v>
+        <v>395</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG54" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="AH54" t="s" s="2">
         <v>43</v>
@@ -7773,35 +7726,35 @@
         <v>87</v>
       </c>
       <c r="AJ54" t="s" s="2">
-        <v>43</v>
+        <v>402</v>
       </c>
       <c r="AK54" t="s" s="2">
-        <v>256</v>
+        <v>403</v>
       </c>
       <c r="AL54" t="s" s="2">
-        <v>257</v>
+        <v>404</v>
       </c>
       <c r="AM54" t="s" s="2">
-        <v>43</v>
+        <v>405</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>362</v>
+        <v>406</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
-        <v>363</v>
+        <v>407</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" t="s" s="2">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="F55" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G55" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="H55" t="s" s="2">
         <v>43</v>
@@ -7810,17 +7763,19 @@
         <v>53</v>
       </c>
       <c r="J55" t="s" s="2">
-        <v>364</v>
+        <v>408</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>365</v>
+        <v>409</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>366</v>
-      </c>
-      <c r="M55" s="2"/>
+        <v>410</v>
+      </c>
+      <c r="M55" t="s" s="2">
+        <v>411</v>
+      </c>
       <c r="N55" t="s" s="2">
-        <v>367</v>
+        <v>401</v>
       </c>
       <c r="O55" t="s" s="2">
         <v>43</v>
@@ -7869,13 +7824,13 @@
         <v>43</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>362</v>
+        <v>406</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG55" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="AH55" t="s" s="2">
         <v>43</v>
@@ -7884,32 +7839,32 @@
         <v>87</v>
       </c>
       <c r="AJ55" t="s" s="2">
-        <v>368</v>
+        <v>402</v>
       </c>
       <c r="AK55" t="s" s="2">
-        <v>369</v>
+        <v>412</v>
       </c>
       <c r="AL55" t="s" s="2">
-        <v>370</v>
+        <v>404</v>
       </c>
       <c r="AM55" t="s" s="2">
-        <v>371</v>
+        <v>405</v>
       </c>
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>372</v>
+        <v>413</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
-        <v>373</v>
+        <v>43</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F56" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G56" t="s" s="2">
         <v>43</v>
@@ -7918,22 +7873,22 @@
         <v>43</v>
       </c>
       <c r="I56" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="J56" t="s" s="2">
-        <v>374</v>
+        <v>414</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>375</v>
+        <v>415</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>376</v>
+        <v>416</v>
       </c>
       <c r="M56" t="s" s="2">
-        <v>377</v>
+        <v>417</v>
       </c>
       <c r="N56" t="s" s="2">
-        <v>378</v>
+        <v>418</v>
       </c>
       <c r="O56" t="s" s="2">
         <v>43</v>
@@ -7982,13 +7937,13 @@
         <v>43</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>372</v>
+        <v>413</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG56" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="AH56" t="s" s="2">
         <v>43</v>
@@ -7997,32 +7952,32 @@
         <v>87</v>
       </c>
       <c r="AJ56" t="s" s="2">
-        <v>379</v>
+        <v>43</v>
       </c>
       <c r="AK56" t="s" s="2">
-        <v>380</v>
+        <v>419</v>
       </c>
       <c r="AL56" t="s" s="2">
-        <v>381</v>
+        <v>362</v>
       </c>
       <c r="AM56" t="s" s="2">
-        <v>382</v>
+        <v>43</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="2">
-        <v>383</v>
+        <v>420</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
-        <v>384</v>
+        <v>421</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" t="s" s="2">
         <v>52</v>
       </c>
       <c r="F57" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G57" t="s" s="2">
         <v>53</v>
@@ -8031,22 +7986,22 @@
         <v>43</v>
       </c>
       <c r="I57" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="J57" t="s" s="2">
-        <v>385</v>
+        <v>422</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>386</v>
+        <v>423</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>387</v>
+        <v>424</v>
       </c>
       <c r="M57" t="s" s="2">
-        <v>388</v>
+        <v>425</v>
       </c>
       <c r="N57" t="s" s="2">
-        <v>389</v>
+        <v>426</v>
       </c>
       <c r="O57" t="s" s="2">
         <v>43</v>
@@ -8095,13 +8050,13 @@
         <v>43</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>383</v>
+        <v>420</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG57" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="AH57" t="s" s="2">
         <v>43</v>
@@ -8110,25 +8065,25 @@
         <v>87</v>
       </c>
       <c r="AJ57" t="s" s="2">
-        <v>390</v>
+        <v>43</v>
       </c>
       <c r="AK57" t="s" s="2">
-        <v>391</v>
+        <v>427</v>
       </c>
       <c r="AL57" t="s" s="2">
-        <v>392</v>
+        <v>428</v>
       </c>
       <c r="AM57" t="s" s="2">
-        <v>393</v>
+        <v>43</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>394</v>
+        <v>429</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
-        <v>395</v>
+        <v>43</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" t="s" s="2">
@@ -8138,29 +8093,25 @@
         <v>52</v>
       </c>
       <c r="G58" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="H58" t="s" s="2">
         <v>43</v>
       </c>
       <c r="I58" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="J58" t="s" s="2">
-        <v>89</v>
+        <v>54</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>396</v>
+        <v>66</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>397</v>
-      </c>
-      <c r="M58" t="s" s="2">
-        <v>398</v>
-      </c>
-      <c r="N58" t="s" s="2">
-        <v>399</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="M58" s="2"/>
+      <c r="N58" s="2"/>
       <c r="O58" t="s" s="2">
         <v>43</v>
       </c>
@@ -8208,7 +8159,7 @@
         <v>43</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>394</v>
+        <v>68</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>41</v>
@@ -8220,60 +8171,58 @@
         <v>43</v>
       </c>
       <c r="AI58" t="s" s="2">
-        <v>87</v>
+        <v>43</v>
       </c>
       <c r="AJ58" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK58" t="s" s="2">
-        <v>400</v>
+        <v>43</v>
       </c>
       <c r="AL58" t="s" s="2">
-        <v>401</v>
+        <v>69</v>
       </c>
       <c r="AM58" t="s" s="2">
-        <v>402</v>
+        <v>43</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>403</v>
+        <v>430</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
-        <v>404</v>
+        <v>71</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" t="s" s="2">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="F59" t="s" s="2">
         <v>42</v>
       </c>
       <c r="G59" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="H59" t="s" s="2">
         <v>43</v>
       </c>
       <c r="I59" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="J59" t="s" s="2">
-        <v>405</v>
+        <v>72</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>406</v>
+        <v>73</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>407</v>
+        <v>74</v>
       </c>
       <c r="M59" t="s" s="2">
-        <v>408</v>
-      </c>
-      <c r="N59" t="s" s="2">
-        <v>409</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="N59" s="2"/>
       <c r="O59" t="s" s="2">
         <v>43</v>
       </c>
@@ -8309,19 +8258,19 @@
         <v>43</v>
       </c>
       <c r="AA59" t="s" s="2">
-        <v>43</v>
+        <v>76</v>
       </c>
       <c r="AB59" t="s" s="2">
-        <v>43</v>
+        <v>77</v>
       </c>
       <c r="AC59" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AD59" t="s" s="2">
-        <v>43</v>
+        <v>78</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>403</v>
+        <v>79</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>41</v>
@@ -8333,35 +8282,35 @@
         <v>43</v>
       </c>
       <c r="AI59" t="s" s="2">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="AJ59" t="s" s="2">
-        <v>410</v>
+        <v>43</v>
       </c>
       <c r="AK59" t="s" s="2">
-        <v>411</v>
+        <v>43</v>
       </c>
       <c r="AL59" t="s" s="2">
-        <v>412</v>
+        <v>69</v>
       </c>
       <c r="AM59" t="s" s="2">
-        <v>413</v>
+        <v>43</v>
       </c>
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>414</v>
+        <v>431</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
-        <v>415</v>
+        <v>43</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" t="s" s="2">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="F60" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="G60" t="s" s="2">
         <v>43</v>
@@ -8373,20 +8322,18 @@
         <v>53</v>
       </c>
       <c r="J60" t="s" s="2">
-        <v>416</v>
+        <v>54</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>417</v>
+        <v>303</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>418</v>
+        <v>304</v>
       </c>
       <c r="M60" t="s" s="2">
-        <v>419</v>
-      </c>
-      <c r="N60" t="s" s="2">
-        <v>409</v>
-      </c>
+        <v>305</v>
+      </c>
+      <c r="N60" s="2"/>
       <c r="O60" t="s" s="2">
         <v>43</v>
       </c>
@@ -8434,36 +8381,36 @@
         <v>43</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>414</v>
+        <v>306</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG60" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="AH60" t="s" s="2">
-        <v>43</v>
+        <v>307</v>
       </c>
       <c r="AI60" t="s" s="2">
         <v>87</v>
       </c>
       <c r="AJ60" t="s" s="2">
-        <v>410</v>
+        <v>43</v>
       </c>
       <c r="AK60" t="s" s="2">
-        <v>420</v>
+        <v>43</v>
       </c>
       <c r="AL60" t="s" s="2">
-        <v>412</v>
+        <v>153</v>
       </c>
       <c r="AM60" t="s" s="2">
-        <v>413</v>
+        <v>43</v>
       </c>
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>421</v>
+        <v>432</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
@@ -8474,7 +8421,7 @@
         <v>41</v>
       </c>
       <c r="F61" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="G61" t="s" s="2">
         <v>43</v>
@@ -8483,23 +8430,21 @@
         <v>43</v>
       </c>
       <c r="I61" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="J61" t="s" s="2">
-        <v>422</v>
+        <v>95</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>423</v>
+        <v>309</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>424</v>
+        <v>310</v>
       </c>
       <c r="M61" t="s" s="2">
-        <v>425</v>
-      </c>
-      <c r="N61" t="s" s="2">
-        <v>426</v>
-      </c>
+        <v>311</v>
+      </c>
+      <c r="N61" s="2"/>
       <c r="O61" t="s" s="2">
         <v>43</v>
       </c>
@@ -8523,13 +8468,13 @@
         <v>43</v>
       </c>
       <c r="W61" t="s" s="2">
-        <v>43</v>
+        <v>111</v>
       </c>
       <c r="X61" t="s" s="2">
-        <v>43</v>
+        <v>312</v>
       </c>
       <c r="Y61" t="s" s="2">
-        <v>43</v>
+        <v>313</v>
       </c>
       <c r="Z61" t="s" s="2">
         <v>43</v>
@@ -8547,13 +8492,13 @@
         <v>43</v>
       </c>
       <c r="AE61" t="s" s="2">
-        <v>421</v>
+        <v>314</v>
       </c>
       <c r="AF61" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG61" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="AH61" t="s" s="2">
         <v>43</v>
@@ -8565,54 +8510,52 @@
         <v>43</v>
       </c>
       <c r="AK61" t="s" s="2">
-        <v>427</v>
+        <v>43</v>
       </c>
       <c r="AL61" t="s" s="2">
-        <v>370</v>
+        <v>153</v>
       </c>
       <c r="AM61" t="s" s="2">
         <v>43</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>428</v>
+        <v>433</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
-        <v>429</v>
+        <v>43</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" t="s" s="2">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="F62" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="G62" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="H62" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="I62" t="s" s="2">
         <v>53</v>
       </c>
-      <c r="H62" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="I62" t="s" s="2">
-        <v>43</v>
-      </c>
       <c r="J62" t="s" s="2">
-        <v>430</v>
+        <v>164</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>431</v>
+        <v>316</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>432</v>
+        <v>317</v>
       </c>
       <c r="M62" t="s" s="2">
-        <v>433</v>
-      </c>
-      <c r="N62" t="s" s="2">
-        <v>434</v>
-      </c>
+        <v>318</v>
+      </c>
+      <c r="N62" s="2"/>
       <c r="O62" t="s" s="2">
         <v>43</v>
       </c>
@@ -8660,13 +8603,13 @@
         <v>43</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>428</v>
+        <v>319</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG62" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="AH62" t="s" s="2">
         <v>43</v>
@@ -8678,10 +8621,10 @@
         <v>43</v>
       </c>
       <c r="AK62" t="s" s="2">
-        <v>435</v>
+        <v>43</v>
       </c>
       <c r="AL62" t="s" s="2">
-        <v>436</v>
+        <v>320</v>
       </c>
       <c r="AM62" t="s" s="2">
         <v>43</v>
@@ -8689,7 +8632,7 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
@@ -8709,18 +8652,20 @@
         <v>43</v>
       </c>
       <c r="I63" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="J63" t="s" s="2">
         <v>54</v>
       </c>
       <c r="K63" t="s" s="2">
-        <v>66</v>
+        <v>322</v>
       </c>
       <c r="L63" t="s" s="2">
-        <v>67</v>
-      </c>
-      <c r="M63" s="2"/>
+        <v>323</v>
+      </c>
+      <c r="M63" t="s" s="2">
+        <v>324</v>
+      </c>
       <c r="N63" s="2"/>
       <c r="O63" t="s" s="2">
         <v>43</v>
@@ -8769,7 +8714,7 @@
         <v>43</v>
       </c>
       <c r="AE63" t="s" s="2">
-        <v>68</v>
+        <v>325</v>
       </c>
       <c r="AF63" t="s" s="2">
         <v>41</v>
@@ -8781,7 +8726,7 @@
         <v>43</v>
       </c>
       <c r="AI63" t="s" s="2">
-        <v>43</v>
+        <v>87</v>
       </c>
       <c r="AJ63" t="s" s="2">
         <v>43</v>
@@ -8790,7 +8735,7 @@
         <v>43</v>
       </c>
       <c r="AL63" t="s" s="2">
-        <v>69</v>
+        <v>153</v>
       </c>
       <c r="AM63" t="s" s="2">
         <v>43</v>
@@ -8798,11 +8743,11 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" t="s" s="2">
@@ -8821,16 +8766,16 @@
         <v>43</v>
       </c>
       <c r="J64" t="s" s="2">
-        <v>72</v>
+        <v>436</v>
       </c>
       <c r="K64" t="s" s="2">
-        <v>73</v>
+        <v>437</v>
       </c>
       <c r="L64" t="s" s="2">
-        <v>74</v>
+        <v>438</v>
       </c>
       <c r="M64" t="s" s="2">
-        <v>75</v>
+        <v>439</v>
       </c>
       <c r="N64" s="2"/>
       <c r="O64" t="s" s="2">
@@ -8868,19 +8813,19 @@
         <v>43</v>
       </c>
       <c r="AA64" t="s" s="2">
-        <v>76</v>
+        <v>43</v>
       </c>
       <c r="AB64" t="s" s="2">
-        <v>77</v>
+        <v>43</v>
       </c>
       <c r="AC64" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AD64" t="s" s="2">
-        <v>78</v>
+        <v>43</v>
       </c>
       <c r="AE64" t="s" s="2">
-        <v>79</v>
+        <v>435</v>
       </c>
       <c r="AF64" t="s" s="2">
         <v>41</v>
@@ -8892,7 +8837,7 @@
         <v>43</v>
       </c>
       <c r="AI64" t="s" s="2">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="AJ64" t="s" s="2">
         <v>43</v>
@@ -8901,7 +8846,7 @@
         <v>43</v>
       </c>
       <c r="AL64" t="s" s="2">
-        <v>69</v>
+        <v>440</v>
       </c>
       <c r="AM64" t="s" s="2">
         <v>43</v>
@@ -8909,18 +8854,18 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
-        <v>43</v>
+        <v>442</v>
       </c>
       <c r="D65" s="2"/>
       <c r="E65" t="s" s="2">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="F65" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G65" t="s" s="2">
         <v>43</v>
@@ -8932,18 +8877,18 @@
         <v>53</v>
       </c>
       <c r="J65" t="s" s="2">
-        <v>54</v>
+        <v>443</v>
       </c>
       <c r="K65" t="s" s="2">
-        <v>303</v>
+        <v>444</v>
       </c>
       <c r="L65" t="s" s="2">
-        <v>304</v>
-      </c>
-      <c r="M65" t="s" s="2">
-        <v>305</v>
-      </c>
-      <c r="N65" s="2"/>
+        <v>445</v>
+      </c>
+      <c r="M65" s="2"/>
+      <c r="N65" t="s" s="2">
+        <v>446</v>
+      </c>
       <c r="O65" t="s" s="2">
         <v>43</v>
       </c>
@@ -8991,16 +8936,16 @@
         <v>43</v>
       </c>
       <c r="AE65" t="s" s="2">
-        <v>306</v>
+        <v>441</v>
       </c>
       <c r="AF65" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG65" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="AH65" t="s" s="2">
-        <v>307</v>
+        <v>43</v>
       </c>
       <c r="AI65" t="s" s="2">
         <v>87</v>
@@ -9009,10 +8954,10 @@
         <v>43</v>
       </c>
       <c r="AK65" t="s" s="2">
-        <v>43</v>
+        <v>447</v>
       </c>
       <c r="AL65" t="s" s="2">
-        <v>153</v>
+        <v>428</v>
       </c>
       <c r="AM65" t="s" s="2">
         <v>43</v>
@@ -9020,7 +8965,7 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>440</v>
+        <v>448</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
@@ -9040,20 +8985,18 @@
         <v>43</v>
       </c>
       <c r="I66" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="J66" t="s" s="2">
-        <v>95</v>
+        <v>54</v>
       </c>
       <c r="K66" t="s" s="2">
-        <v>309</v>
+        <v>66</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>310</v>
-      </c>
-      <c r="M66" t="s" s="2">
-        <v>311</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="M66" s="2"/>
       <c r="N66" s="2"/>
       <c r="O66" t="s" s="2">
         <v>43</v>
@@ -9078,13 +9021,13 @@
         <v>43</v>
       </c>
       <c r="W66" t="s" s="2">
-        <v>111</v>
+        <v>43</v>
       </c>
       <c r="X66" t="s" s="2">
-        <v>312</v>
+        <v>43</v>
       </c>
       <c r="Y66" t="s" s="2">
-        <v>313</v>
+        <v>43</v>
       </c>
       <c r="Z66" t="s" s="2">
         <v>43</v>
@@ -9102,7 +9045,7 @@
         <v>43</v>
       </c>
       <c r="AE66" t="s" s="2">
-        <v>314</v>
+        <v>68</v>
       </c>
       <c r="AF66" t="s" s="2">
         <v>41</v>
@@ -9114,7 +9057,7 @@
         <v>43</v>
       </c>
       <c r="AI66" t="s" s="2">
-        <v>87</v>
+        <v>43</v>
       </c>
       <c r="AJ66" t="s" s="2">
         <v>43</v>
@@ -9123,7 +9066,7 @@
         <v>43</v>
       </c>
       <c r="AL66" t="s" s="2">
-        <v>153</v>
+        <v>69</v>
       </c>
       <c r="AM66" t="s" s="2">
         <v>43</v>
@@ -9131,18 +9074,18 @@
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>441</v>
+        <v>449</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" t="s" s="2">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="D67" s="2"/>
       <c r="E67" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F67" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G67" t="s" s="2">
         <v>43</v>
@@ -9151,19 +9094,19 @@
         <v>43</v>
       </c>
       <c r="I67" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="J67" t="s" s="2">
-        <v>164</v>
+        <v>72</v>
       </c>
       <c r="K67" t="s" s="2">
-        <v>316</v>
+        <v>73</v>
       </c>
       <c r="L67" t="s" s="2">
-        <v>317</v>
+        <v>74</v>
       </c>
       <c r="M67" t="s" s="2">
-        <v>318</v>
+        <v>75</v>
       </c>
       <c r="N67" s="2"/>
       <c r="O67" t="s" s="2">
@@ -9213,19 +9156,19 @@
         <v>43</v>
       </c>
       <c r="AE67" t="s" s="2">
-        <v>319</v>
+        <v>79</v>
       </c>
       <c r="AF67" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG67" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="AH67" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AI67" t="s" s="2">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="AJ67" t="s" s="2">
         <v>43</v>
@@ -9234,7 +9177,7 @@
         <v>43</v>
       </c>
       <c r="AL67" t="s" s="2">
-        <v>320</v>
+        <v>69</v>
       </c>
       <c r="AM67" t="s" s="2">
         <v>43</v>
@@ -9242,41 +9185,43 @@
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>442</v>
+        <v>450</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" t="s" s="2">
-        <v>43</v>
+        <v>451</v>
       </c>
       <c r="D68" s="2"/>
       <c r="E68" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F68" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G68" t="s" s="2">
         <v>43</v>
       </c>
       <c r="H68" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="I68" t="s" s="2">
         <v>53</v>
       </c>
       <c r="J68" t="s" s="2">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="K68" t="s" s="2">
-        <v>322</v>
+        <v>452</v>
       </c>
       <c r="L68" t="s" s="2">
-        <v>323</v>
+        <v>453</v>
       </c>
       <c r="M68" t="s" s="2">
-        <v>324</v>
-      </c>
-      <c r="N68" s="2"/>
+        <v>75</v>
+      </c>
+      <c r="N68" t="s" s="2">
+        <v>160</v>
+      </c>
       <c r="O68" t="s" s="2">
         <v>43</v>
       </c>
@@ -9324,19 +9269,19 @@
         <v>43</v>
       </c>
       <c r="AE68" t="s" s="2">
-        <v>325</v>
+        <v>454</v>
       </c>
       <c r="AF68" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG68" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="AH68" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AI68" t="s" s="2">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="AJ68" t="s" s="2">
         <v>43</v>
@@ -9353,7 +9298,7 @@
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>443</v>
+        <v>455</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" t="s" s="2">
@@ -9364,7 +9309,7 @@
         <v>41</v>
       </c>
       <c r="F69" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="G69" t="s" s="2">
         <v>43</v>
@@ -9376,18 +9321,20 @@
         <v>43</v>
       </c>
       <c r="J69" t="s" s="2">
-        <v>444</v>
+        <v>54</v>
       </c>
       <c r="K69" t="s" s="2">
-        <v>445</v>
+        <v>456</v>
       </c>
       <c r="L69" t="s" s="2">
-        <v>446</v>
+        <v>457</v>
       </c>
       <c r="M69" t="s" s="2">
-        <v>447</v>
-      </c>
-      <c r="N69" s="2"/>
+        <v>458</v>
+      </c>
+      <c r="N69" t="s" s="2">
+        <v>459</v>
+      </c>
       <c r="O69" t="s" s="2">
         <v>43</v>
       </c>
@@ -9435,13 +9382,13 @@
         <v>43</v>
       </c>
       <c r="AE69" t="s" s="2">
-        <v>443</v>
+        <v>455</v>
       </c>
       <c r="AF69" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG69" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="AH69" t="s" s="2">
         <v>43</v>
@@ -9456,7 +9403,7 @@
         <v>43</v>
       </c>
       <c r="AL69" t="s" s="2">
-        <v>448</v>
+        <v>460</v>
       </c>
       <c r="AM69" t="s" s="2">
         <v>43</v>
@@ -9464,18 +9411,18 @@
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>449</v>
+        <v>461</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" t="s" s="2">
-        <v>450</v>
+        <v>43</v>
       </c>
       <c r="D70" s="2"/>
       <c r="E70" t="s" s="2">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="F70" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="G70" t="s" s="2">
         <v>43</v>
@@ -9487,18 +9434,16 @@
         <v>53</v>
       </c>
       <c r="J70" t="s" s="2">
-        <v>451</v>
+        <v>462</v>
       </c>
       <c r="K70" t="s" s="2">
-        <v>452</v>
+        <v>463</v>
       </c>
       <c r="L70" t="s" s="2">
-        <v>453</v>
+        <v>464</v>
       </c>
       <c r="M70" s="2"/>
-      <c r="N70" t="s" s="2">
-        <v>454</v>
-      </c>
+      <c r="N70" s="2"/>
       <c r="O70" t="s" s="2">
         <v>43</v>
       </c>
@@ -9546,13 +9491,13 @@
         <v>43</v>
       </c>
       <c r="AE70" t="s" s="2">
-        <v>449</v>
+        <v>461</v>
       </c>
       <c r="AF70" t="s" s="2">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="AG70" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="AH70" t="s" s="2">
         <v>43</v>
@@ -9564,22 +9509,22 @@
         <v>43</v>
       </c>
       <c r="AK70" t="s" s="2">
-        <v>455</v>
+        <v>43</v>
       </c>
       <c r="AL70" t="s" s="2">
-        <v>436</v>
+        <v>465</v>
       </c>
       <c r="AM70" t="s" s="2">
         <v>43</v>
       </c>
     </row>
-    <row r="71" hidden="true">
+    <row r="71">
       <c r="A71" t="s" s="2">
-        <v>456</v>
+        <v>466</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" t="s" s="2">
-        <v>43</v>
+        <v>467</v>
       </c>
       <c r="D71" s="2"/>
       <c r="E71" t="s" s="2">
@@ -9589,7 +9534,7 @@
         <v>52</v>
       </c>
       <c r="G71" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="H71" t="s" s="2">
         <v>43</v>
@@ -9601,13 +9546,15 @@
         <v>54</v>
       </c>
       <c r="K71" t="s" s="2">
-        <v>66</v>
+        <v>468</v>
       </c>
       <c r="L71" t="s" s="2">
-        <v>67</v>
+        <v>469</v>
       </c>
       <c r="M71" s="2"/>
-      <c r="N71" s="2"/>
+      <c r="N71" t="s" s="2">
+        <v>470</v>
+      </c>
       <c r="O71" t="s" s="2">
         <v>43</v>
       </c>
@@ -9655,7 +9602,7 @@
         <v>43</v>
       </c>
       <c r="AE71" t="s" s="2">
-        <v>68</v>
+        <v>466</v>
       </c>
       <c r="AF71" t="s" s="2">
         <v>41</v>
@@ -9667,28 +9614,28 @@
         <v>43</v>
       </c>
       <c r="AI71" t="s" s="2">
-        <v>43</v>
+        <v>87</v>
       </c>
       <c r="AJ71" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK71" t="s" s="2">
-        <v>43</v>
+        <v>471</v>
       </c>
       <c r="AL71" t="s" s="2">
-        <v>69</v>
+        <v>472</v>
       </c>
       <c r="AM71" t="s" s="2">
         <v>43</v>
       </c>
     </row>
-    <row r="72" hidden="true">
+    <row r="72">
       <c r="A72" t="s" s="2">
-        <v>457</v>
+        <v>473</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" t="s" s="2">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="D72" s="2"/>
       <c r="E72" t="s" s="2">
@@ -9698,7 +9645,7 @@
         <v>42</v>
       </c>
       <c r="G72" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="H72" t="s" s="2">
         <v>43</v>
@@ -9707,17 +9654,15 @@
         <v>43</v>
       </c>
       <c r="J72" t="s" s="2">
-        <v>72</v>
+        <v>190</v>
       </c>
       <c r="K72" t="s" s="2">
-        <v>73</v>
+        <v>474</v>
       </c>
       <c r="L72" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="M72" t="s" s="2">
-        <v>75</v>
-      </c>
+        <v>475</v>
+      </c>
+      <c r="M72" s="2"/>
       <c r="N72" s="2"/>
       <c r="O72" t="s" s="2">
         <v>43</v>
@@ -9742,13 +9687,11 @@
         <v>43</v>
       </c>
       <c r="W72" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="X72" t="s" s="2">
-        <v>43</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="X72" s="2"/>
       <c r="Y72" t="s" s="2">
-        <v>43</v>
+        <v>476</v>
       </c>
       <c r="Z72" t="s" s="2">
         <v>43</v>
@@ -9766,7 +9709,7 @@
         <v>43</v>
       </c>
       <c r="AE72" t="s" s="2">
-        <v>79</v>
+        <v>473</v>
       </c>
       <c r="AF72" t="s" s="2">
         <v>41</v>
@@ -9778,28 +9721,28 @@
         <v>43</v>
       </c>
       <c r="AI72" t="s" s="2">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="AJ72" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK72" t="s" s="2">
-        <v>43</v>
+        <v>471</v>
       </c>
       <c r="AL72" t="s" s="2">
-        <v>69</v>
+        <v>477</v>
       </c>
       <c r="AM72" t="s" s="2">
         <v>43</v>
       </c>
     </row>
-    <row r="73" hidden="true">
+    <row r="73">
       <c r="A73" t="s" s="2">
-        <v>458</v>
+        <v>478</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" t="s" s="2">
-        <v>459</v>
+        <v>43</v>
       </c>
       <c r="D73" s="2"/>
       <c r="E73" t="s" s="2">
@@ -9809,28 +9752,28 @@
         <v>42</v>
       </c>
       <c r="G73" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="H73" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="I73" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="J73" t="s" s="2">
-        <v>72</v>
+        <v>479</v>
       </c>
       <c r="K73" t="s" s="2">
-        <v>460</v>
+        <v>480</v>
       </c>
       <c r="L73" t="s" s="2">
-        <v>461</v>
+        <v>481</v>
       </c>
       <c r="M73" t="s" s="2">
-        <v>75</v>
+        <v>482</v>
       </c>
       <c r="N73" t="s" s="2">
-        <v>160</v>
+        <v>483</v>
       </c>
       <c r="O73" t="s" s="2">
         <v>43</v>
@@ -9879,7 +9822,7 @@
         <v>43</v>
       </c>
       <c r="AE73" t="s" s="2">
-        <v>462</v>
+        <v>478</v>
       </c>
       <c r="AF73" t="s" s="2">
         <v>41</v>
@@ -9891,1137 +9834,23 @@
         <v>43</v>
       </c>
       <c r="AI73" t="s" s="2">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="AJ73" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK73" t="s" s="2">
-        <v>43</v>
+        <v>471</v>
       </c>
       <c r="AL73" t="s" s="2">
-        <v>153</v>
+        <v>484</v>
       </c>
       <c r="AM73" t="s" s="2">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="74" hidden="true">
-      <c r="A74" t="s" s="2">
-        <v>463</v>
-      </c>
-      <c r="B74" s="2"/>
-      <c r="C74" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="D74" s="2"/>
-      <c r="E74" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="F74" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="G74" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="H74" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="I74" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="J74" t="s" s="2">
-        <v>54</v>
-      </c>
-      <c r="K74" t="s" s="2">
-        <v>464</v>
-      </c>
-      <c r="L74" t="s" s="2">
-        <v>465</v>
-      </c>
-      <c r="M74" t="s" s="2">
-        <v>466</v>
-      </c>
-      <c r="N74" t="s" s="2">
-        <v>467</v>
-      </c>
-      <c r="O74" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="P74" s="2"/>
-      <c r="Q74" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="R74" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="S74" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="T74" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="U74" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="V74" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="W74" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="X74" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="Y74" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="Z74" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AA74" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AB74" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AC74" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AD74" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AE74" t="s" s="2">
-        <v>463</v>
-      </c>
-      <c r="AF74" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG74" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AH74" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AI74" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="AJ74" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AK74" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AL74" t="s" s="2">
-        <v>468</v>
-      </c>
-      <c r="AM74" t="s" s="2">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="75" hidden="true">
-      <c r="A75" t="s" s="2">
-        <v>469</v>
-      </c>
-      <c r="B75" s="2"/>
-      <c r="C75" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="D75" s="2"/>
-      <c r="E75" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="F75" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="G75" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="H75" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="I75" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="J75" t="s" s="2">
-        <v>470</v>
-      </c>
-      <c r="K75" t="s" s="2">
-        <v>471</v>
-      </c>
-      <c r="L75" t="s" s="2">
-        <v>472</v>
-      </c>
-      <c r="M75" s="2"/>
-      <c r="N75" s="2"/>
-      <c r="O75" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="P75" s="2"/>
-      <c r="Q75" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="R75" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="S75" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="T75" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="U75" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="V75" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="W75" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="X75" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="Y75" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="Z75" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AA75" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AB75" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AC75" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AD75" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AE75" t="s" s="2">
-        <v>469</v>
-      </c>
-      <c r="AF75" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AG75" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AH75" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AI75" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="AJ75" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AK75" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AL75" t="s" s="2">
-        <v>473</v>
-      </c>
-      <c r="AM75" t="s" s="2">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="s" s="2">
-        <v>474</v>
-      </c>
-      <c r="B76" s="2"/>
-      <c r="C76" t="s" s="2">
-        <v>475</v>
-      </c>
-      <c r="D76" s="2"/>
-      <c r="E76" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="F76" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="G76" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="H76" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="I76" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="J76" t="s" s="2">
-        <v>54</v>
-      </c>
-      <c r="K76" t="s" s="2">
-        <v>476</v>
-      </c>
-      <c r="L76" t="s" s="2">
-        <v>477</v>
-      </c>
-      <c r="M76" s="2"/>
-      <c r="N76" t="s" s="2">
-        <v>478</v>
-      </c>
-      <c r="O76" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="P76" s="2"/>
-      <c r="Q76" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="R76" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="S76" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="T76" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="U76" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="V76" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="W76" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="X76" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="Y76" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="Z76" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AA76" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AB76" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AC76" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AD76" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AE76" t="s" s="2">
-        <v>474</v>
-      </c>
-      <c r="AF76" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG76" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AH76" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AI76" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="AJ76" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AK76" t="s" s="2">
-        <v>479</v>
-      </c>
-      <c r="AL76" t="s" s="2">
-        <v>480</v>
-      </c>
-      <c r="AM76" t="s" s="2">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="s" s="2">
-        <v>481</v>
-      </c>
-      <c r="B77" s="2"/>
-      <c r="C77" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="D77" s="2"/>
-      <c r="E77" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="F77" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="G77" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="H77" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="I77" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="J77" t="s" s="2">
-        <v>190</v>
-      </c>
-      <c r="K77" t="s" s="2">
-        <v>482</v>
-      </c>
-      <c r="L77" t="s" s="2">
-        <v>483</v>
-      </c>
-      <c r="M77" s="2"/>
-      <c r="N77" s="2"/>
-      <c r="O77" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="P77" s="2"/>
-      <c r="Q77" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="R77" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="S77" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="T77" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="U77" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="V77" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="W77" t="s" s="2">
-        <v>119</v>
-      </c>
-      <c r="X77" t="s" s="2">
-        <v>484</v>
-      </c>
-      <c r="Y77" t="s" s="2">
-        <v>485</v>
-      </c>
-      <c r="Z77" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AA77" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AB77" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AC77" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AD77" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AE77" t="s" s="2">
-        <v>481</v>
-      </c>
-      <c r="AF77" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG77" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AH77" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AI77" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="AJ77" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AK77" t="s" s="2">
-        <v>479</v>
-      </c>
-      <c r="AL77" t="s" s="2">
-        <v>486</v>
-      </c>
-      <c r="AM77" t="s" s="2">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="78" hidden="true">
-      <c r="A78" t="s" s="2">
-        <v>487</v>
-      </c>
-      <c r="B78" s="2"/>
-      <c r="C78" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="D78" s="2"/>
-      <c r="E78" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="F78" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="G78" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="H78" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="I78" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="J78" t="s" s="2">
-        <v>54</v>
-      </c>
-      <c r="K78" t="s" s="2">
-        <v>66</v>
-      </c>
-      <c r="L78" t="s" s="2">
-        <v>67</v>
-      </c>
-      <c r="M78" s="2"/>
-      <c r="N78" s="2"/>
-      <c r="O78" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="P78" s="2"/>
-      <c r="Q78" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="R78" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="S78" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="T78" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="U78" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="V78" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="W78" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="X78" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="Y78" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="Z78" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AA78" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AB78" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AC78" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AD78" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AE78" t="s" s="2">
-        <v>68</v>
-      </c>
-      <c r="AF78" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG78" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AH78" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AI78" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AJ78" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AK78" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AL78" t="s" s="2">
-        <v>69</v>
-      </c>
-      <c r="AM78" t="s" s="2">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="79" hidden="true">
-      <c r="A79" t="s" s="2">
-        <v>488</v>
-      </c>
-      <c r="B79" s="2"/>
-      <c r="C79" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="D79" s="2"/>
-      <c r="E79" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="F79" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="G79" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="H79" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="I79" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="J79" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="K79" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="L79" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="M79" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="N79" s="2"/>
-      <c r="O79" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="P79" s="2"/>
-      <c r="Q79" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="R79" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="S79" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="T79" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="U79" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="V79" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="W79" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="X79" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="Y79" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="Z79" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AA79" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AB79" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AC79" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AD79" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AE79" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AF79" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG79" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AH79" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AI79" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AJ79" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AK79" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AL79" t="s" s="2">
-        <v>69</v>
-      </c>
-      <c r="AM79" t="s" s="2">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="80" hidden="true">
-      <c r="A80" t="s" s="2">
-        <v>489</v>
-      </c>
-      <c r="B80" s="2"/>
-      <c r="C80" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="D80" s="2"/>
-      <c r="E80" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="F80" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="G80" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="H80" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="I80" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="J80" t="s" s="2">
-        <v>107</v>
-      </c>
-      <c r="K80" t="s" s="2">
-        <v>201</v>
-      </c>
-      <c r="L80" t="s" s="2">
-        <v>202</v>
-      </c>
-      <c r="M80" t="s" s="2">
-        <v>203</v>
-      </c>
-      <c r="N80" t="s" s="2">
-        <v>204</v>
-      </c>
-      <c r="O80" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="P80" s="2"/>
-      <c r="Q80" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="R80" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="S80" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="T80" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="U80" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="V80" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="W80" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="X80" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="Y80" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="Z80" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AA80" t="s" s="2">
-        <v>490</v>
-      </c>
-      <c r="AB80" s="2"/>
-      <c r="AC80" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AD80" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AE80" t="s" s="2">
-        <v>205</v>
-      </c>
-      <c r="AF80" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG80" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AH80" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AI80" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="AJ80" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AK80" t="s" s="2">
-        <v>206</v>
-      </c>
-      <c r="AL80" t="s" s="2">
-        <v>207</v>
-      </c>
-      <c r="AM80" t="s" s="2">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="81" hidden="true">
-      <c r="A81" t="s" s="2">
-        <v>489</v>
-      </c>
-      <c r="B81" t="s" s="2">
-        <v>491</v>
-      </c>
-      <c r="C81" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="D81" s="2"/>
-      <c r="E81" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="F81" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="G81" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="H81" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="I81" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="J81" t="s" s="2">
-        <v>107</v>
-      </c>
-      <c r="K81" t="s" s="2">
-        <v>492</v>
-      </c>
-      <c r="L81" t="s" s="2">
-        <v>202</v>
-      </c>
-      <c r="M81" t="s" s="2">
-        <v>203</v>
-      </c>
-      <c r="N81" t="s" s="2">
-        <v>204</v>
-      </c>
-      <c r="O81" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="P81" s="2"/>
-      <c r="Q81" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="R81" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="S81" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="T81" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="U81" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="V81" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="W81" t="s" s="2">
-        <v>184</v>
-      </c>
-      <c r="X81" t="s" s="2">
-        <v>492</v>
-      </c>
-      <c r="Y81" t="s" s="2">
-        <v>493</v>
-      </c>
-      <c r="Z81" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AA81" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AB81" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AC81" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AD81" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AE81" t="s" s="2">
-        <v>205</v>
-      </c>
-      <c r="AF81" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG81" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AH81" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AI81" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="AJ81" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AK81" t="s" s="2">
-        <v>206</v>
-      </c>
-      <c r="AL81" t="s" s="2">
-        <v>207</v>
-      </c>
-      <c r="AM81" t="s" s="2">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="82" hidden="true">
-      <c r="A82" t="s" s="2">
-        <v>494</v>
-      </c>
-      <c r="B82" s="2"/>
-      <c r="C82" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="D82" s="2"/>
-      <c r="E82" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="F82" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="G82" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="H82" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="I82" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="J82" t="s" s="2">
-        <v>54</v>
-      </c>
-      <c r="K82" t="s" s="2">
-        <v>251</v>
-      </c>
-      <c r="L82" t="s" s="2">
-        <v>252</v>
-      </c>
-      <c r="M82" t="s" s="2">
-        <v>253</v>
-      </c>
-      <c r="N82" t="s" s="2">
-        <v>254</v>
-      </c>
-      <c r="O82" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="P82" s="2"/>
-      <c r="Q82" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="R82" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="S82" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="T82" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="U82" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="V82" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="W82" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="X82" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="Y82" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="Z82" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AA82" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AB82" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AC82" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AD82" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AE82" t="s" s="2">
-        <v>255</v>
-      </c>
-      <c r="AF82" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG82" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AH82" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AI82" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="AJ82" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AK82" t="s" s="2">
-        <v>256</v>
-      </c>
-      <c r="AL82" t="s" s="2">
-        <v>257</v>
-      </c>
-      <c r="AM82" t="s" s="2">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="s" s="2">
-        <v>495</v>
-      </c>
-      <c r="B83" s="2"/>
-      <c r="C83" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="D83" s="2"/>
-      <c r="E83" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="F83" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="G83" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="H83" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="I83" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="J83" t="s" s="2">
-        <v>496</v>
-      </c>
-      <c r="K83" t="s" s="2">
-        <v>497</v>
-      </c>
-      <c r="L83" t="s" s="2">
-        <v>498</v>
-      </c>
-      <c r="M83" t="s" s="2">
-        <v>499</v>
-      </c>
-      <c r="N83" t="s" s="2">
-        <v>500</v>
-      </c>
-      <c r="O83" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="P83" s="2"/>
-      <c r="Q83" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="R83" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="S83" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="T83" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="U83" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="V83" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="W83" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="X83" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="Y83" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="Z83" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AA83" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AB83" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AC83" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AD83" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AE83" t="s" s="2">
-        <v>495</v>
-      </c>
-      <c r="AF83" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG83" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AH83" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AI83" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="AJ83" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AK83" t="s" s="2">
-        <v>479</v>
-      </c>
-      <c r="AL83" t="s" s="2">
-        <v>501</v>
-      </c>
-      <c r="AM83" t="s" s="2">
         <v>43</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AM83">
+  <autoFilter ref="A1:AM73">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -11031,7 +9860,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI82">
+  <conditionalFormatting sqref="A2:AI72">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>

<commit_message>
SNOMED Imaging procedure fix - updated code with preferred binding SNOMED Imaging procedure fix - updated known issues
</commit_message>
<xml_diff>
--- a/output/DiagnosticReport/diagnosticreport-imag-atomic-1.xlsx
+++ b/output/DiagnosticReport/diagnosticreport-imag-atomic-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2564" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2563" uniqueCount="484">
   <si>
     <t>Path</t>
   </si>
@@ -1099,10 +1099,7 @@
     <t>A code or name that describes this diagnostic report.</t>
   </si>
   <si>
-    <t>Codes that describe Diagnostic Reports.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/report-codes</t>
+    <t>https://healthterminologies.gov.au/fhir/ValueSet/imaging-procedure-1</t>
   </si>
   <si>
     <t>Event.code</t>
@@ -7126,11 +7123,9 @@
       <c r="W49" t="s" s="2">
         <v>134</v>
       </c>
-      <c r="X49" t="s" s="2">
+      <c r="X49" s="2"/>
+      <c r="Y49" t="s" s="2">
         <v>348</v>
-      </c>
-      <c r="Y49" t="s" s="2">
-        <v>349</v>
       </c>
       <c r="Z49" t="s" s="2">
         <v>43</v>
@@ -7163,25 +7158,25 @@
         <v>87</v>
       </c>
       <c r="AJ49" t="s" s="2">
+        <v>349</v>
+      </c>
+      <c r="AK49" t="s" s="2">
         <v>350</v>
       </c>
-      <c r="AK49" t="s" s="2">
+      <c r="AL49" t="s" s="2">
         <v>351</v>
       </c>
-      <c r="AL49" t="s" s="2">
+      <c r="AM49" t="s" s="2">
         <v>352</v>
-      </c>
-      <c r="AM49" t="s" s="2">
-        <v>353</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="2">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" t="s" s="2">
@@ -7200,17 +7195,17 @@
         <v>53</v>
       </c>
       <c r="J50" t="s" s="2">
+        <v>355</v>
+      </c>
+      <c r="K50" t="s" s="2">
         <v>356</v>
       </c>
-      <c r="K50" t="s" s="2">
+      <c r="L50" t="s" s="2">
         <v>357</v>
-      </c>
-      <c r="L50" t="s" s="2">
-        <v>358</v>
       </c>
       <c r="M50" s="2"/>
       <c r="N50" t="s" s="2">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="O50" t="s" s="2">
         <v>43</v>
@@ -7259,7 +7254,7 @@
         <v>43</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>41</v>
@@ -7274,25 +7269,25 @@
         <v>87</v>
       </c>
       <c r="AJ50" t="s" s="2">
+        <v>359</v>
+      </c>
+      <c r="AK50" t="s" s="2">
         <v>360</v>
       </c>
-      <c r="AK50" t="s" s="2">
+      <c r="AL50" t="s" s="2">
         <v>361</v>
       </c>
-      <c r="AL50" t="s" s="2">
+      <c r="AM50" t="s" s="2">
         <v>362</v>
-      </c>
-      <c r="AM50" t="s" s="2">
-        <v>363</v>
       </c>
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" t="s" s="2">
@@ -7311,19 +7306,19 @@
         <v>53</v>
       </c>
       <c r="J51" t="s" s="2">
+        <v>365</v>
+      </c>
+      <c r="K51" t="s" s="2">
         <v>366</v>
       </c>
-      <c r="K51" t="s" s="2">
+      <c r="L51" t="s" s="2">
         <v>367</v>
       </c>
-      <c r="L51" t="s" s="2">
+      <c r="M51" t="s" s="2">
         <v>368</v>
       </c>
-      <c r="M51" t="s" s="2">
+      <c r="N51" t="s" s="2">
         <v>369</v>
-      </c>
-      <c r="N51" t="s" s="2">
-        <v>370</v>
       </c>
       <c r="O51" t="s" s="2">
         <v>43</v>
@@ -7372,7 +7367,7 @@
         <v>43</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>41</v>
@@ -7387,25 +7382,25 @@
         <v>87</v>
       </c>
       <c r="AJ51" t="s" s="2">
+        <v>370</v>
+      </c>
+      <c r="AK51" t="s" s="2">
         <v>371</v>
       </c>
-      <c r="AK51" t="s" s="2">
+      <c r="AL51" t="s" s="2">
         <v>372</v>
       </c>
-      <c r="AL51" t="s" s="2">
+      <c r="AM51" t="s" s="2">
         <v>373</v>
-      </c>
-      <c r="AM51" t="s" s="2">
-        <v>374</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="2">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" t="s" s="2">
@@ -7424,19 +7419,19 @@
         <v>53</v>
       </c>
       <c r="J52" t="s" s="2">
+        <v>376</v>
+      </c>
+      <c r="K52" t="s" s="2">
         <v>377</v>
       </c>
-      <c r="K52" t="s" s="2">
+      <c r="L52" t="s" s="2">
         <v>378</v>
       </c>
-      <c r="L52" t="s" s="2">
+      <c r="M52" t="s" s="2">
         <v>379</v>
       </c>
-      <c r="M52" t="s" s="2">
+      <c r="N52" t="s" s="2">
         <v>380</v>
-      </c>
-      <c r="N52" t="s" s="2">
-        <v>381</v>
       </c>
       <c r="O52" t="s" s="2">
         <v>43</v>
@@ -7485,7 +7480,7 @@
         <v>43</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>41</v>
@@ -7500,25 +7495,25 @@
         <v>87</v>
       </c>
       <c r="AJ52" t="s" s="2">
+        <v>381</v>
+      </c>
+      <c r="AK52" t="s" s="2">
         <v>382</v>
       </c>
-      <c r="AK52" t="s" s="2">
+      <c r="AL52" t="s" s="2">
         <v>383</v>
       </c>
-      <c r="AL52" t="s" s="2">
+      <c r="AM52" t="s" s="2">
         <v>384</v>
-      </c>
-      <c r="AM52" t="s" s="2">
-        <v>385</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="2">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" t="s" s="2">
@@ -7540,16 +7535,16 @@
         <v>89</v>
       </c>
       <c r="K53" t="s" s="2">
+        <v>387</v>
+      </c>
+      <c r="L53" t="s" s="2">
         <v>388</v>
       </c>
-      <c r="L53" t="s" s="2">
+      <c r="M53" t="s" s="2">
         <v>389</v>
       </c>
-      <c r="M53" t="s" s="2">
+      <c r="N53" t="s" s="2">
         <v>390</v>
-      </c>
-      <c r="N53" t="s" s="2">
-        <v>391</v>
       </c>
       <c r="O53" t="s" s="2">
         <v>43</v>
@@ -7598,7 +7593,7 @@
         <v>43</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>41</v>
@@ -7616,22 +7611,22 @@
         <v>43</v>
       </c>
       <c r="AK53" t="s" s="2">
+        <v>391</v>
+      </c>
+      <c r="AL53" t="s" s="2">
         <v>392</v>
       </c>
-      <c r="AL53" t="s" s="2">
+      <c r="AM53" t="s" s="2">
         <v>393</v>
-      </c>
-      <c r="AM53" t="s" s="2">
-        <v>394</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="2">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" t="s" s="2">
@@ -7650,19 +7645,19 @@
         <v>53</v>
       </c>
       <c r="J54" t="s" s="2">
+        <v>396</v>
+      </c>
+      <c r="K54" t="s" s="2">
         <v>397</v>
       </c>
-      <c r="K54" t="s" s="2">
+      <c r="L54" t="s" s="2">
         <v>398</v>
       </c>
-      <c r="L54" t="s" s="2">
+      <c r="M54" t="s" s="2">
         <v>399</v>
       </c>
-      <c r="M54" t="s" s="2">
+      <c r="N54" t="s" s="2">
         <v>400</v>
-      </c>
-      <c r="N54" t="s" s="2">
-        <v>401</v>
       </c>
       <c r="O54" t="s" s="2">
         <v>43</v>
@@ -7711,7 +7706,7 @@
         <v>43</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>41</v>
@@ -7726,25 +7721,25 @@
         <v>87</v>
       </c>
       <c r="AJ54" t="s" s="2">
+        <v>401</v>
+      </c>
+      <c r="AK54" t="s" s="2">
         <v>402</v>
       </c>
-      <c r="AK54" t="s" s="2">
+      <c r="AL54" t="s" s="2">
         <v>403</v>
       </c>
-      <c r="AL54" t="s" s="2">
+      <c r="AM54" t="s" s="2">
         <v>404</v>
-      </c>
-      <c r="AM54" t="s" s="2">
-        <v>405</v>
       </c>
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" t="s" s="2">
@@ -7763,19 +7758,19 @@
         <v>53</v>
       </c>
       <c r="J55" t="s" s="2">
+        <v>407</v>
+      </c>
+      <c r="K55" t="s" s="2">
         <v>408</v>
       </c>
-      <c r="K55" t="s" s="2">
+      <c r="L55" t="s" s="2">
         <v>409</v>
       </c>
-      <c r="L55" t="s" s="2">
+      <c r="M55" t="s" s="2">
         <v>410</v>
       </c>
-      <c r="M55" t="s" s="2">
-        <v>411</v>
-      </c>
       <c r="N55" t="s" s="2">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="O55" t="s" s="2">
         <v>43</v>
@@ -7824,7 +7819,7 @@
         <v>43</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>41</v>
@@ -7839,21 +7834,21 @@
         <v>87</v>
       </c>
       <c r="AJ55" t="s" s="2">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="AK55" t="s" s="2">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="AL55" t="s" s="2">
+        <v>403</v>
+      </c>
+      <c r="AM55" t="s" s="2">
         <v>404</v>
-      </c>
-      <c r="AM55" t="s" s="2">
-        <v>405</v>
       </c>
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
@@ -7876,19 +7871,19 @@
         <v>43</v>
       </c>
       <c r="J56" t="s" s="2">
+        <v>413</v>
+      </c>
+      <c r="K56" t="s" s="2">
         <v>414</v>
       </c>
-      <c r="K56" t="s" s="2">
+      <c r="L56" t="s" s="2">
         <v>415</v>
       </c>
-      <c r="L56" t="s" s="2">
+      <c r="M56" t="s" s="2">
         <v>416</v>
       </c>
-      <c r="M56" t="s" s="2">
+      <c r="N56" t="s" s="2">
         <v>417</v>
-      </c>
-      <c r="N56" t="s" s="2">
-        <v>418</v>
       </c>
       <c r="O56" t="s" s="2">
         <v>43</v>
@@ -7937,7 +7932,7 @@
         <v>43</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>41</v>
@@ -7955,10 +7950,10 @@
         <v>43</v>
       </c>
       <c r="AK56" t="s" s="2">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="AL56" t="s" s="2">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="AM56" t="s" s="2">
         <v>43</v>
@@ -7966,11 +7961,11 @@
     </row>
     <row r="57">
       <c r="A57" t="s" s="2">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" t="s" s="2">
@@ -7989,19 +7984,19 @@
         <v>43</v>
       </c>
       <c r="J57" t="s" s="2">
+        <v>421</v>
+      </c>
+      <c r="K57" t="s" s="2">
         <v>422</v>
       </c>
-      <c r="K57" t="s" s="2">
+      <c r="L57" t="s" s="2">
         <v>423</v>
       </c>
-      <c r="L57" t="s" s="2">
+      <c r="M57" t="s" s="2">
         <v>424</v>
       </c>
-      <c r="M57" t="s" s="2">
+      <c r="N57" t="s" s="2">
         <v>425</v>
-      </c>
-      <c r="N57" t="s" s="2">
-        <v>426</v>
       </c>
       <c r="O57" t="s" s="2">
         <v>43</v>
@@ -8050,7 +8045,7 @@
         <v>43</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>41</v>
@@ -8068,10 +8063,10 @@
         <v>43</v>
       </c>
       <c r="AK57" t="s" s="2">
+        <v>426</v>
+      </c>
+      <c r="AL57" t="s" s="2">
         <v>427</v>
-      </c>
-      <c r="AL57" t="s" s="2">
-        <v>428</v>
       </c>
       <c r="AM57" t="s" s="2">
         <v>43</v>
@@ -8079,7 +8074,7 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
@@ -8188,7 +8183,7 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
@@ -8299,7 +8294,7 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
@@ -8410,7 +8405,7 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
@@ -8521,7 +8516,7 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
@@ -8632,7 +8627,7 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
@@ -8743,7 +8738,7 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
@@ -8766,16 +8761,16 @@
         <v>43</v>
       </c>
       <c r="J64" t="s" s="2">
+        <v>435</v>
+      </c>
+      <c r="K64" t="s" s="2">
         <v>436</v>
       </c>
-      <c r="K64" t="s" s="2">
+      <c r="L64" t="s" s="2">
         <v>437</v>
       </c>
-      <c r="L64" t="s" s="2">
+      <c r="M64" t="s" s="2">
         <v>438</v>
-      </c>
-      <c r="M64" t="s" s="2">
-        <v>439</v>
       </c>
       <c r="N64" s="2"/>
       <c r="O64" t="s" s="2">
@@ -8825,7 +8820,7 @@
         <v>43</v>
       </c>
       <c r="AE64" t="s" s="2">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="AF64" t="s" s="2">
         <v>41</v>
@@ -8846,7 +8841,7 @@
         <v>43</v>
       </c>
       <c r="AL64" t="s" s="2">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="AM64" t="s" s="2">
         <v>43</v>
@@ -8854,11 +8849,11 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D65" s="2"/>
       <c r="E65" t="s" s="2">
@@ -8877,17 +8872,17 @@
         <v>53</v>
       </c>
       <c r="J65" t="s" s="2">
+        <v>442</v>
+      </c>
+      <c r="K65" t="s" s="2">
         <v>443</v>
       </c>
-      <c r="K65" t="s" s="2">
+      <c r="L65" t="s" s="2">
         <v>444</v>
-      </c>
-      <c r="L65" t="s" s="2">
-        <v>445</v>
       </c>
       <c r="M65" s="2"/>
       <c r="N65" t="s" s="2">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="O65" t="s" s="2">
         <v>43</v>
@@ -8936,7 +8931,7 @@
         <v>43</v>
       </c>
       <c r="AE65" t="s" s="2">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="AF65" t="s" s="2">
         <v>41</v>
@@ -8954,10 +8949,10 @@
         <v>43</v>
       </c>
       <c r="AK65" t="s" s="2">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="AL65" t="s" s="2">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="AM65" t="s" s="2">
         <v>43</v>
@@ -8965,7 +8960,7 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
@@ -9074,7 +9069,7 @@
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" t="s" s="2">
@@ -9185,11 +9180,11 @@
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" t="s" s="2">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D68" s="2"/>
       <c r="E68" t="s" s="2">
@@ -9211,10 +9206,10 @@
         <v>72</v>
       </c>
       <c r="K68" t="s" s="2">
+        <v>451</v>
+      </c>
+      <c r="L68" t="s" s="2">
         <v>452</v>
-      </c>
-      <c r="L68" t="s" s="2">
-        <v>453</v>
       </c>
       <c r="M68" t="s" s="2">
         <v>75</v>
@@ -9269,7 +9264,7 @@
         <v>43</v>
       </c>
       <c r="AE68" t="s" s="2">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="AF68" t="s" s="2">
         <v>41</v>
@@ -9298,7 +9293,7 @@
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" t="s" s="2">
@@ -9324,16 +9319,16 @@
         <v>54</v>
       </c>
       <c r="K69" t="s" s="2">
+        <v>455</v>
+      </c>
+      <c r="L69" t="s" s="2">
         <v>456</v>
       </c>
-      <c r="L69" t="s" s="2">
+      <c r="M69" t="s" s="2">
         <v>457</v>
       </c>
-      <c r="M69" t="s" s="2">
+      <c r="N69" t="s" s="2">
         <v>458</v>
-      </c>
-      <c r="N69" t="s" s="2">
-        <v>459</v>
       </c>
       <c r="O69" t="s" s="2">
         <v>43</v>
@@ -9382,7 +9377,7 @@
         <v>43</v>
       </c>
       <c r="AE69" t="s" s="2">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="AF69" t="s" s="2">
         <v>41</v>
@@ -9403,7 +9398,7 @@
         <v>43</v>
       </c>
       <c r="AL69" t="s" s="2">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="AM69" t="s" s="2">
         <v>43</v>
@@ -9411,7 +9406,7 @@
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" t="s" s="2">
@@ -9434,13 +9429,13 @@
         <v>53</v>
       </c>
       <c r="J70" t="s" s="2">
+        <v>461</v>
+      </c>
+      <c r="K70" t="s" s="2">
         <v>462</v>
       </c>
-      <c r="K70" t="s" s="2">
+      <c r="L70" t="s" s="2">
         <v>463</v>
-      </c>
-      <c r="L70" t="s" s="2">
-        <v>464</v>
       </c>
       <c r="M70" s="2"/>
       <c r="N70" s="2"/>
@@ -9491,7 +9486,7 @@
         <v>43</v>
       </c>
       <c r="AE70" t="s" s="2">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="AF70" t="s" s="2">
         <v>52</v>
@@ -9512,7 +9507,7 @@
         <v>43</v>
       </c>
       <c r="AL70" t="s" s="2">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="AM70" t="s" s="2">
         <v>43</v>
@@ -9520,11 +9515,11 @@
     </row>
     <row r="71">
       <c r="A71" t="s" s="2">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" t="s" s="2">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D71" s="2"/>
       <c r="E71" t="s" s="2">
@@ -9546,14 +9541,14 @@
         <v>54</v>
       </c>
       <c r="K71" t="s" s="2">
+        <v>467</v>
+      </c>
+      <c r="L71" t="s" s="2">
         <v>468</v>
-      </c>
-      <c r="L71" t="s" s="2">
-        <v>469</v>
       </c>
       <c r="M71" s="2"/>
       <c r="N71" t="s" s="2">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="O71" t="s" s="2">
         <v>43</v>
@@ -9602,7 +9597,7 @@
         <v>43</v>
       </c>
       <c r="AE71" t="s" s="2">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="AF71" t="s" s="2">
         <v>41</v>
@@ -9620,10 +9615,10 @@
         <v>43</v>
       </c>
       <c r="AK71" t="s" s="2">
+        <v>470</v>
+      </c>
+      <c r="AL71" t="s" s="2">
         <v>471</v>
-      </c>
-      <c r="AL71" t="s" s="2">
-        <v>472</v>
       </c>
       <c r="AM71" t="s" s="2">
         <v>43</v>
@@ -9631,7 +9626,7 @@
     </row>
     <row r="72">
       <c r="A72" t="s" s="2">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" t="s" s="2">
@@ -9657,10 +9652,10 @@
         <v>190</v>
       </c>
       <c r="K72" t="s" s="2">
+        <v>473</v>
+      </c>
+      <c r="L72" t="s" s="2">
         <v>474</v>
-      </c>
-      <c r="L72" t="s" s="2">
-        <v>475</v>
       </c>
       <c r="M72" s="2"/>
       <c r="N72" s="2"/>
@@ -9691,7 +9686,7 @@
       </c>
       <c r="X72" s="2"/>
       <c r="Y72" t="s" s="2">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="Z72" t="s" s="2">
         <v>43</v>
@@ -9709,7 +9704,7 @@
         <v>43</v>
       </c>
       <c r="AE72" t="s" s="2">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="AF72" t="s" s="2">
         <v>41</v>
@@ -9727,10 +9722,10 @@
         <v>43</v>
       </c>
       <c r="AK72" t="s" s="2">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="AL72" t="s" s="2">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="AM72" t="s" s="2">
         <v>43</v>
@@ -9738,7 +9733,7 @@
     </row>
     <row r="73">
       <c r="A73" t="s" s="2">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" t="s" s="2">
@@ -9761,19 +9756,19 @@
         <v>43</v>
       </c>
       <c r="J73" t="s" s="2">
+        <v>478</v>
+      </c>
+      <c r="K73" t="s" s="2">
         <v>479</v>
       </c>
-      <c r="K73" t="s" s="2">
+      <c r="L73" t="s" s="2">
         <v>480</v>
       </c>
-      <c r="L73" t="s" s="2">
+      <c r="M73" t="s" s="2">
         <v>481</v>
       </c>
-      <c r="M73" t="s" s="2">
+      <c r="N73" t="s" s="2">
         <v>482</v>
-      </c>
-      <c r="N73" t="s" s="2">
-        <v>483</v>
       </c>
       <c r="O73" t="s" s="2">
         <v>43</v>
@@ -9822,7 +9817,7 @@
         <v>43</v>
       </c>
       <c r="AE73" t="s" s="2">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="AF73" t="s" s="2">
         <v>41</v>
@@ -9840,10 +9835,10 @@
         <v>43</v>
       </c>
       <c r="AK73" t="s" s="2">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="AL73" t="s" s="2">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="AM73" t="s" s="2">
         <v>43</v>

</xml_diff>